<commit_message>
USD 3M YC bootstrap - fix rates
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YC3MBootstrapping.xlsx
@@ -17,7 +17,6 @@
   <definedNames>
     <definedName name="Accuracy">'General Settings'!$D$23</definedName>
     <definedName name="BondBasisDayCounter">'General Settings'!$M$13</definedName>
-    <definedName name="Calendar" localSheetId="5">'General Settings'!#REF!</definedName>
     <definedName name="Calendar">'General Settings'!$D$18</definedName>
     <definedName name="Conventions" localSheetId="5">'3M_Swaps'!$P$6:$R$10</definedName>
     <definedName name="Currency">'General Settings'!$D$4</definedName>
@@ -605,12 +604,6 @@
     <t>USD_YC3MRH_FUT3MZ5</t>
   </si>
   <si>
-    <t>USD_YC3MRH_FUT3MH6</t>
-  </si>
-  <si>
-    <t>USD_YC3MRH_FUT3MM6</t>
-  </si>
-  <si>
     <t>USD_YC3MRH_AM3L3Y</t>
   </si>
   <si>
@@ -777,6 +770,12 @@
   </si>
   <si>
     <t>USD_YCRH_Swaps</t>
+  </si>
+  <si>
+    <t>USD_YC3MRH_FUT3MU4</t>
+  </si>
+  <si>
+    <t>USD_YC3MRH_FUT3MZ4</t>
   </si>
 </sst>
 </file>
@@ -904,7 +903,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,12 +956,6 @@
       <patternFill patternType="gray0625">
         <fgColor indexed="22"/>
         <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1413,7 +1406,7 @@
     <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1813,9 +1806,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="10" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1831,21 +1836,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="10" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2164,39 +2154,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="187" customWidth="1"/>
-    <col min="3" max="3" width="18" style="187" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="187" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="187" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2.7109375" style="187" customWidth="1"/>
-    <col min="8" max="9" width="8" style="187"/>
-    <col min="10" max="11" width="2.7109375" style="187" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="187" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53.7109375" style="187" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" style="187" customWidth="1"/>
-    <col min="15" max="16384" width="8" style="187"/>
+    <col min="1" max="2" width="2.7109375" style="181" customWidth="1"/>
+    <col min="3" max="3" width="18" style="181" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="181" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="181" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2.7109375" style="181" customWidth="1"/>
+    <col min="8" max="9" width="8" style="181"/>
+    <col min="10" max="11" width="2.7109375" style="181" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="181" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.7109375" style="181" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="181" customWidth="1"/>
+    <col min="15" max="16384" width="8" style="181"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="187" t="str">
+      <c r="B1" s="181" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Dec  5 2013 11:03:51</v>
+        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Jan 15 2014 16:53:36</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="189" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="197"/>
-      <c r="K2" s="195" t="s">
-        <v>162</v>
-      </c>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="190"/>
+      <c r="F2" s="191"/>
+      <c r="K2" s="189" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="190"/>
+      <c r="M2" s="190"/>
+      <c r="N2" s="190"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="60"/>
@@ -2219,13 +2209,13 @@
       </c>
       <c r="E4" s="57"/>
       <c r="F4" s="56"/>
-      <c r="H4" s="190" t="s">
+      <c r="H4" s="184" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="191"/>
+      <c r="I4" s="185"/>
       <c r="K4" s="127"/>
       <c r="L4" s="126" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M4" s="120" t="b">
         <v>1</v>
@@ -2242,19 +2232,19 @@
       </c>
       <c r="E5" s="57"/>
       <c r="F5" s="56"/>
-      <c r="H5" s="188" t="s">
+      <c r="H5" s="182" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="189" t="s">
+      <c r="I5" s="183" t="s">
         <v>111</v>
       </c>
       <c r="K5" s="127"/>
       <c r="L5" s="126" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="M5" s="128" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data2\XML\</v>
+        <v>C:\erik\repos\quantlib\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="N5" s="125"/>
     </row>
@@ -2269,15 +2259,15 @@
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="56"/>
-      <c r="H6" s="188" t="s">
+      <c r="H6" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="189" t="s">
+      <c r="I6" s="183" t="s">
         <v>108</v>
       </c>
       <c r="K6" s="127"/>
       <c r="L6" s="126" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M6" s="117" t="b">
         <v>1</v>
@@ -2295,10 +2285,10 @@
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="56"/>
-      <c r="H7" s="188" t="s">
+      <c r="H7" s="182" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="189"/>
+      <c r="I7" s="183"/>
       <c r="K7" s="124"/>
       <c r="L7" s="123"/>
       <c r="M7" s="123"/>
@@ -2315,16 +2305,16 @@
       </c>
       <c r="E8" s="57"/>
       <c r="F8" s="56"/>
-      <c r="H8" s="192" t="s">
+      <c r="H8" s="186" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="193" t="s">
+      <c r="I8" s="187" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="194"/>
-      <c r="L8" s="194"/>
-      <c r="M8" s="194"/>
-      <c r="N8" s="194"/>
+      <c r="K8" s="188"/>
+      <c r="L8" s="188"/>
+      <c r="M8" s="188"/>
+      <c r="N8" s="188"/>
     </row>
     <row r="9" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="60"/>
@@ -2337,12 +2327,12 @@
       </c>
       <c r="E9" s="57"/>
       <c r="F9" s="56"/>
-      <c r="K9" s="195" t="s">
-        <v>158</v>
-      </c>
-      <c r="L9" s="196"/>
-      <c r="M9" s="196"/>
-      <c r="N9" s="196"/>
+      <c r="K9" s="189" t="s">
+        <v>156</v>
+      </c>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="60"/>
@@ -2365,16 +2355,16 @@
         <v>100</v>
       </c>
       <c r="D11" s="85">
-        <v>41654.209652777776</v>
+        <v>41654.758842592593</v>
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="56"/>
       <c r="K11" s="119"/>
       <c r="L11" s="118" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M11" s="120" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N11" s="116"/>
     </row>
@@ -2390,10 +2380,10 @@
       <c r="F12" s="56"/>
       <c r="K12" s="119"/>
       <c r="L12" s="118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M12" s="117" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N12" s="116"/>
     </row>
@@ -2405,10 +2395,10 @@
       <c r="F13" s="56"/>
       <c r="K13" s="119"/>
       <c r="L13" s="118" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M13" s="120" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N13" s="116"/>
     </row>
@@ -2419,16 +2409,16 @@
       </c>
       <c r="D14" s="82" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYC3M#0009</v>
+        <v>_USDYC3M#0002</v>
       </c>
       <c r="E14" s="57"/>
       <c r="F14" s="56"/>
       <c r="K14" s="119"/>
       <c r="L14" s="118" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M14" s="120" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="N14" s="116"/>
     </row>
@@ -2445,7 +2435,7 @@
       <c r="F15" s="56"/>
       <c r="K15" s="119"/>
       <c r="L15" s="118" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M15" s="120" t="str">
         <f>PROPER(Currency)&amp;"YC"</f>
@@ -2466,7 +2456,7 @@
       <c r="F16" s="56"/>
       <c r="K16" s="119"/>
       <c r="L16" s="118" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M16" s="120" t="str">
         <f>PROPER(Currency)&amp;"YCSTD"</f>
@@ -2598,9 +2588,9 @@
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
         <v>41656</v>
       </c>
-      <c r="D27" s="63" t="e">
+      <c r="D27" s="63">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="56"/>
@@ -2611,9 +2601,9 @@
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
         <v>59918</v>
       </c>
-      <c r="D28" s="61" t="e">
+      <c r="D28" s="61">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>0.16094323852142145</v>
       </c>
       <c r="E28" s="57"/>
       <c r="F28" s="56"/>
@@ -2624,8 +2614,8 @@
         <v>76</v>
       </c>
       <c r="D29" s="58" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 7th iteration: failed at 14th alive instrument, maturity January 17th, 2017, reference date January 17th, 2014: root not bracketed: f[0.0809127,0.976545] -&gt; [-5.446828e-001,-2.273666e-003]</v>
+        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v/>
       </c>
       <c r="E29" s="57"/>
       <c r="F29" s="56"/>
@@ -2681,7 +2671,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2704,11 +2696,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="192" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="183"/>
-      <c r="D1" s="184"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="194"/>
       <c r="E1" s="31" t="s">
         <v>74</v>
       </c>
@@ -4016,7 +4008,7 @@
       </c>
       <c r="E36" s="14" t="str">
         <f>'3M_Futures'!I3</f>
-        <v>USD_YC3MRH_FUT3MF4#0008</v>
+        <v>USD_YC3MRH_FUT3MF4#0002</v>
       </c>
       <c r="F36" s="28">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -4061,11 +4053,11 @@
       </c>
       <c r="E37" s="14" t="str">
         <f>'3M_Futures'!I4</f>
-        <v>USD_YC3MRH_FUT3MG4#0008</v>
+        <v>USD_YC3MRH_FUT3MG4#0002</v>
       </c>
       <c r="F37" s="28">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
-        <v>99.747500000000002</v>
+        <v>99.754999999999995</v>
       </c>
       <c r="G37" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E37,Trigger)</f>
@@ -4106,11 +4098,11 @@
       </c>
       <c r="E38" s="14" t="str">
         <f>'3M_Futures'!I5</f>
-        <v>USD_YC3MRH_FUT3MH4#0008</v>
+        <v>USD_YC3MRH_FUT3MH4#0002</v>
       </c>
       <c r="F38" s="28">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
-        <v>99.737499999999997</v>
+        <v>99.747500000000002</v>
       </c>
       <c r="G38" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E38,Trigger)</f>
@@ -4151,11 +4143,11 @@
       </c>
       <c r="E39" s="14" t="str">
         <f>'3M_Futures'!I6</f>
-        <v>USD_YC3MRH_FUT3MJ4#0008</v>
+        <v>USD_YC3MRH_FUT3MJ4#0002</v>
       </c>
       <c r="F39" s="28">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
-        <v>99.727499999999992</v>
+        <v>99.74</v>
       </c>
       <c r="G39" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E39,Trigger)</f>
@@ -4196,11 +4188,11 @@
       </c>
       <c r="E40" s="14" t="str">
         <f>'3M_Futures'!I7</f>
-        <v>USD_YC3MRH_FUT3MK4#0008</v>
+        <v>USD_YC3MRH_FUT3MK4#0002</v>
       </c>
       <c r="F40" s="28">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
-        <v>99.707499999999996</v>
+        <v>99.724999999999994</v>
       </c>
       <c r="G40" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E40,Trigger)</f>
@@ -4241,11 +4233,11 @@
       </c>
       <c r="E41" s="14" t="str">
         <f>'3M_Futures'!I8</f>
-        <v>USD_YC3MRH_FUT3MM4#0008</v>
+        <v>USD_YC3MRH_FUT3MM4#0002</v>
       </c>
       <c r="F41" s="28">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
-        <v>99.694999999999993</v>
+        <v>99.707499999999996</v>
       </c>
       <c r="G41" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E41,Trigger)</f>
@@ -4286,18 +4278,18 @@
       </c>
       <c r="E42" s="14" t="str">
         <f>'3M_Futures'!I9</f>
-        <v>USD_YC3MRH_FUT3MN4#0008</v>
-      </c>
-      <c r="F42" s="28" t="e">
+        <v>USD_YC3MRH_FUT3MN4#0002</v>
+      </c>
+      <c r="F42" s="28">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G42" s="13" t="e">
+        <v>99.692499999999995</v>
+      </c>
+      <c r="G42" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E42,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H42" s="181" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H42" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="I42" s="12">
         <v>60</v>
@@ -4331,7 +4323,7 @@
       </c>
       <c r="E43" s="14" t="str">
         <f>'3M_Futures'!I10</f>
-        <v>USD_YC3MRH_FUT3MQ4#0008</v>
+        <v>USD_YC3MRH_FUT3MQ4#0002</v>
       </c>
       <c r="F43" s="28">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4376,18 +4368,18 @@
       </c>
       <c r="E44" s="14" t="str">
         <f>'3M_Futures'!I11</f>
-        <v>USD_YC3MRH_FUT3MU4#0008</v>
-      </c>
-      <c r="F44" s="28" t="e">
+        <v>USD_YC3MRH_FUT3MU4#0002</v>
+      </c>
+      <c r="F44" s="28">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G44" s="13" t="e">
+        <v>99.647499999999994</v>
+      </c>
+      <c r="G44" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E44,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H44" s="181" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H44" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="I44" s="12">
         <v>60</v>
@@ -4421,7 +4413,7 @@
       </c>
       <c r="E45" s="14" t="str">
         <f>'3M_Futures'!I12</f>
-        <v>USD_YC3MRH_FUT3MV4#0008</v>
+        <v>USD_YC3MRH_FUT3MV4#0002</v>
       </c>
       <c r="F45" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4431,8 +4423,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H45" s="181" t="b">
-        <v>0</v>
+      <c r="H45" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="I45" s="12">
         <v>60</v>
@@ -4466,7 +4458,7 @@
       </c>
       <c r="E46" s="14" t="str">
         <f>'3M_Futures'!I13</f>
-        <v>USD_YC3MRH_FUT3MX4#0008</v>
+        <v>USD_YC3MRH_FUT3MX4#0002</v>
       </c>
       <c r="F46" s="28">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
@@ -4511,18 +4503,18 @@
       </c>
       <c r="E47" s="14" t="str">
         <f>'3M_Futures'!I14</f>
-        <v>USD_YC3MRH_FUT3MZ4#0008</v>
-      </c>
-      <c r="F47" s="28" t="e">
+        <v>USD_YC3MRH_FUT3MZ4#0002</v>
+      </c>
+      <c r="F47" s="28">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G47" s="13" t="e">
+        <v>99.5625</v>
+      </c>
+      <c r="G47" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E47,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H47" s="181" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H47" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="I47" s="12">
         <v>60</v>
@@ -4556,11 +4548,11 @@
       </c>
       <c r="E48" s="14" t="str">
         <f>'3M_Futures'!I15</f>
-        <v>USD_YC3MRH_FUT3MH5#0008</v>
+        <v>USD_YC3MRH_FUT3MH5#0002</v>
       </c>
       <c r="F48" s="28">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
-        <v>99.537499999999994</v>
+        <v>99.4375</v>
       </c>
       <c r="G48" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E48,Trigger)</f>
@@ -4601,11 +4593,11 @@
       </c>
       <c r="E49" s="14" t="str">
         <f>'3M_Futures'!I16</f>
-        <v>USD_YC3MRH_FUT3MM5#0008</v>
+        <v>USD_YC3MRH_FUT3MM5#0002</v>
       </c>
       <c r="F49" s="28">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
-        <v>99.4375</v>
+        <v>99.272499999999994</v>
       </c>
       <c r="G49" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E49,Trigger)</f>
@@ -4646,11 +4638,11 @@
       </c>
       <c r="E50" s="14" t="str">
         <f>'3M_Futures'!I17</f>
-        <v>USD_YC3MRH_FUT3MU5#0008</v>
+        <v>USD_YC3MRH_FUT3MU5#0002</v>
       </c>
       <c r="F50" s="28">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
-        <v>99.32</v>
+        <v>99.067499999999995</v>
       </c>
       <c r="G50" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E50,Trigger)</f>
@@ -4691,11 +4683,11 @@
       </c>
       <c r="E51" s="14" t="str">
         <f>'3M_Futures'!I18</f>
-        <v>USD_YC3MRH_FUT3MZ5#0008</v>
+        <v>USD_YC3MRH_FUT3MZ5#0002</v>
       </c>
       <c r="F51" s="28">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
-        <v>99.177500000000009</v>
+        <v>98.822500000000005</v>
       </c>
       <c r="G51" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E51,Trigger)</f>
@@ -4736,11 +4728,11 @@
       </c>
       <c r="E52" s="14" t="str">
         <f>'3M_Futures'!I19</f>
-        <v>USD_YC3MRH_FUT3MH6#0008</v>
+        <v>USD_YC3MRH_FUT3MH6#0002</v>
       </c>
       <c r="F52" s="28">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
-        <v>98.992500000000007</v>
+        <v>98.537499999999994</v>
       </c>
       <c r="G52" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E52,Trigger)</f>
@@ -4781,11 +4773,11 @@
       </c>
       <c r="E53" s="14" t="str">
         <f>'3M_Futures'!I20</f>
-        <v>USD_YC3MRH_FUT3MM6#0008</v>
+        <v>USD_YC3MRH_FUT3MM6#0002</v>
       </c>
       <c r="F53" s="28">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
-        <v>98.775000000000006</v>
+        <v>98.242500000000007</v>
       </c>
       <c r="G53" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E53,Trigger)</f>
@@ -4826,11 +4818,11 @@
       </c>
       <c r="E54" s="14" t="str">
         <f>'3M_Futures'!I21</f>
-        <v>USD_YC3MRH_FUT3MU6#0008</v>
+        <v>USD_YC3MRH_FUT3MU6#0002</v>
       </c>
       <c r="F54" s="28">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
-        <v>98.537499999999994</v>
+        <v>97.957499999999996</v>
       </c>
       <c r="G54" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E54,Trigger)</f>
@@ -4871,11 +4863,11 @@
       </c>
       <c r="E55" s="14" t="str">
         <f>'3M_Futures'!I22</f>
-        <v>USD_YC3MRH_FUT3MZ6#0008</v>
+        <v>USD_YC3MRH_FUT3MZ6#0002</v>
       </c>
       <c r="F55" s="28">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
-        <v>98.277500000000003</v>
+        <v>97.682500000000005</v>
       </c>
       <c r="G55" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E55,Trigger)</f>
@@ -4916,11 +4908,11 @@
       </c>
       <c r="E56" s="14" t="str">
         <f>'3M_Futures'!I23</f>
-        <v>USD_YC3MRH_FUT3MH7#0008</v>
+        <v>USD_YC3MRH_FUT3MH7#0002</v>
       </c>
       <c r="F56" s="28">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
-        <v>98.022500000000008</v>
+        <v>97.432500000000005</v>
       </c>
       <c r="G56" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E56,Trigger)</f>
@@ -4961,11 +4953,11 @@
       </c>
       <c r="E57" s="14" t="str">
         <f>'3M_Futures'!I24</f>
-        <v>USD_YC3MRH_FUT3MM7#0008</v>
+        <v>USD_YC3MRH_FUT3MM7#0002</v>
       </c>
       <c r="F57" s="28">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
-        <v>97.792500000000004</v>
+        <v>97.177499999999995</v>
       </c>
       <c r="G57" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E57,Trigger)</f>
@@ -5006,11 +4998,11 @@
       </c>
       <c r="E58" s="14" t="str">
         <f>'3M_Futures'!I25</f>
-        <v>USD_YC3MRH_FUT3MU7#0008</v>
+        <v>USD_YC3MRH_FUT3MU7#0002</v>
       </c>
       <c r="F58" s="28">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
-        <v>97.557500000000005</v>
+        <v>96.952500000000001</v>
       </c>
       <c r="G58" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E58,Trigger)</f>
@@ -5051,11 +5043,11 @@
       </c>
       <c r="E59" s="14" t="str">
         <f>'3M_Futures'!I26</f>
-        <v>USD_YC3MRH_FUT3MZ7#0008</v>
+        <v>USD_YC3MRH_FUT3MZ7#0002</v>
       </c>
       <c r="F59" s="28">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
-        <v>97.337500000000006</v>
+        <v>96.732500000000002</v>
       </c>
       <c r="G59" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E59,Trigger)</f>
@@ -5096,11 +5088,11 @@
       </c>
       <c r="E60" s="14" t="str">
         <f>'3M_Futures'!I27</f>
-        <v>USD_YC3MRH_FUT3MH8#0008</v>
+        <v>USD_YC3MRH_FUT3MH8#0002</v>
       </c>
       <c r="F60" s="28">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
-        <v>97.115000000000009</v>
+        <v>96.542500000000004</v>
       </c>
       <c r="G60" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E60,Trigger)</f>
@@ -5141,11 +5133,11 @@
       </c>
       <c r="E61" s="14" t="str">
         <f>'3M_Futures'!I28</f>
-        <v>USD_YC3MRH_FUT3MM8#0008</v>
+        <v>USD_YC3MRH_FUT3MM8#0002</v>
       </c>
       <c r="F61" s="28">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
-        <v>96.927500000000009</v>
+        <v>96.364999999999995</v>
       </c>
       <c r="G61" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E61,Trigger)</f>
@@ -5186,11 +5178,11 @@
       </c>
       <c r="E62" s="14" t="str">
         <f>'3M_Futures'!I29</f>
-        <v>USD_YC3MRH_FUT3MU8#0008</v>
+        <v>USD_YC3MRH_FUT3MU8#0002</v>
       </c>
       <c r="F62" s="28">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
-        <v>96.747500000000002</v>
+        <v>96.202500000000001</v>
       </c>
       <c r="G62" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E62,Trigger)</f>
@@ -5231,11 +5223,11 @@
       </c>
       <c r="E63" s="14" t="str">
         <f>'3M_Futures'!I30</f>
-        <v>USD_YC3MRH_FUT3MZ8#0008</v>
+        <v>USD_YC3MRH_FUT3MZ8#0002</v>
       </c>
       <c r="F63" s="28">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>96.587500000000006</v>
+        <v>96.052499999999995</v>
       </c>
       <c r="G63" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E63,Trigger)</f>
@@ -5276,11 +5268,11 @@
       </c>
       <c r="E64" s="14" t="str">
         <f>'3M_Futures'!I31</f>
-        <v>USD_YC3MRH_FUT3MH9#0008</v>
+        <v>USD_YC3MRH_FUT3MH9#0002</v>
       </c>
       <c r="F64" s="28">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
-        <v>96.4375</v>
+        <v>95.93</v>
       </c>
       <c r="G64" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E64,Trigger)</f>
@@ -5321,11 +5313,11 @@
       </c>
       <c r="E65" s="14" t="str">
         <f>'3M_Futures'!I32</f>
-        <v>USD_YC3MRH_FUT3MM9#0008</v>
+        <v>USD_YC3MRH_FUT3MM9#0002</v>
       </c>
       <c r="F65" s="28">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
-        <v>96.31</v>
+        <v>95.814999999999998</v>
       </c>
       <c r="G65" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E65,Trigger)</f>
@@ -5366,11 +5358,11 @@
       </c>
       <c r="E66" s="14" t="str">
         <f>'3M_Futures'!I33</f>
-        <v>USD_YC3MRH_FUT3MU9#0008</v>
+        <v>USD_YC3MRH_FUT3MU9#0002</v>
       </c>
       <c r="F66" s="28">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
-        <v>96.192499999999995</v>
+        <v>95.704999999999998</v>
       </c>
       <c r="G66" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E66,Trigger)</f>
@@ -5411,11 +5403,11 @@
       </c>
       <c r="E67" s="14" t="str">
         <f>'3M_Futures'!I34</f>
-        <v>USD_YC3MRH_FUT3MZ9#0008</v>
+        <v>USD_YC3MRH_FUT3MZ9#0002</v>
       </c>
       <c r="F67" s="28">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
-        <v>96.082499999999996</v>
+        <v>95.602500000000006</v>
       </c>
       <c r="G67" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E67,Trigger)</f>
@@ -5456,11 +5448,11 @@
       </c>
       <c r="E68" s="14" t="str">
         <f>'3M_Futures'!I35</f>
-        <v>USD_YC3MRH_FUT3MH0#0008</v>
+        <v>USD_YC3MRH_FUT3MH0#0002</v>
       </c>
       <c r="F68" s="28">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
-        <v>95.97999999999999</v>
+        <v>95.525000000000006</v>
       </c>
       <c r="G68" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E68,Trigger)</f>
@@ -5501,11 +5493,11 @@
       </c>
       <c r="E69" s="14" t="str">
         <f>'3M_Futures'!I36</f>
-        <v>USD_YC3MRH_FUT3MM0#0008</v>
+        <v>USD_YC3MRH_FUT3MM0#0002</v>
       </c>
       <c r="F69" s="28">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
-        <v>95.9</v>
+        <v>95.452500000000001</v>
       </c>
       <c r="G69" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E69,Trigger)</f>
@@ -5546,11 +5538,11 @@
       </c>
       <c r="E70" s="14" t="str">
         <f>'3M_Futures'!I37</f>
-        <v>USD_YC3MRH_FUT3MU0#0008</v>
+        <v>USD_YC3MRH_FUT3MU0#0002</v>
       </c>
       <c r="F70" s="28">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
-        <v>95.822499999999991</v>
+        <v>95.385000000000005</v>
       </c>
       <c r="G70" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E70,Trigger)</f>
@@ -5591,11 +5583,11 @@
       </c>
       <c r="E71" s="14" t="str">
         <f>'3M_Futures'!I38</f>
-        <v>USD_YC3MRH_FUT3MZ0#0008</v>
+        <v>USD_YC3MRH_FUT3MZ0#0002</v>
       </c>
       <c r="F71" s="28">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
-        <v>95.754999999999995</v>
+        <v>95.317499999999995</v>
       </c>
       <c r="G71" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E71,Trigger)</f>
@@ -5636,11 +5628,11 @@
       </c>
       <c r="E72" s="14" t="str">
         <f>'3M_Futures'!I39</f>
-        <v>USD_YC3MRH_FUT3MH1#0008</v>
+        <v>USD_YC3MRH_FUT3MH1#0002</v>
       </c>
       <c r="F72" s="28">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
-        <v>95.69</v>
+        <v>95.277500000000003</v>
       </c>
       <c r="G72" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E72,Trigger)</f>
@@ -5681,11 +5673,11 @@
       </c>
       <c r="E73" s="14" t="str">
         <f>'3M_Futures'!I40</f>
-        <v>USD_YC3MRH_FUT3MM1#0008</v>
+        <v>USD_YC3MRH_FUT3MM1#0002</v>
       </c>
       <c r="F73" s="28">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
-        <v>95.657499999999999</v>
+        <v>95.224999999999994</v>
       </c>
       <c r="G73" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E73,Trigger)</f>
@@ -5726,11 +5718,11 @@
       </c>
       <c r="E74" s="14" t="str">
         <f>'3M_Futures'!I41</f>
-        <v>USD_YC3MRH_FUT3MU1#0008</v>
+        <v>USD_YC3MRH_FUT3MU1#0002</v>
       </c>
       <c r="F74" s="28">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
-        <v>95.594999999999999</v>
+        <v>95.192499999999995</v>
       </c>
       <c r="G74" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E74,Trigger)</f>
@@ -5771,11 +5763,11 @@
       </c>
       <c r="E75" s="14" t="str">
         <f>'3M_Futures'!I42</f>
-        <v>USD_YC3MRH_FUT3MZ1#0008</v>
+        <v>USD_YC3MRH_FUT3MZ1#0002</v>
       </c>
       <c r="F75" s="28">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
-        <v>95.6</v>
+        <v>95.137500000000003</v>
       </c>
       <c r="G75" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E75,Trigger)</f>
@@ -5816,11 +5808,11 @@
       </c>
       <c r="E76" s="14" t="str">
         <f>'3M_Futures'!I43</f>
-        <v>USD_YC3MRH_FUT3MH2#0008</v>
+        <v>USD_YC3MRH_FUT3MH2#0002</v>
       </c>
       <c r="F76" s="28">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
-        <v>95.555000000000007</v>
+        <v>95.117500000000007</v>
       </c>
       <c r="G76" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E76,Trigger)</f>
@@ -5861,11 +5853,11 @@
       </c>
       <c r="E77" s="7" t="str">
         <f>'3M_Futures'!I44</f>
-        <v>USD_YC3MRH_FUT3MM2#0008</v>
+        <v>USD_YC3MRH_FUT3MM2#0002</v>
       </c>
       <c r="F77" s="27">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
-        <v>95.504999999999995</v>
+        <v>95.092500000000001</v>
       </c>
       <c r="G77" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E77,Trigger)</f>
@@ -9872,10 +9864,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="195" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="196"/>
       <c r="D1" s="52" t="s">
         <v>83</v>
       </c>
@@ -9889,9 +9881,9 @@
       <c r="H1" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="32" t="e">
+      <c r="I1" s="32">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -9921,14 +9913,14 @@
         <f>_xll.qlRateHelperLatestDate($D2)</f>
         <v>41663</v>
       </c>
-      <c r="I2" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I2" s="32">
+        <v>0.99994927201790285</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>117</v>
       </c>
       <c r="L2" s="26">
-        <v>2.6090000000000002E-3</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -9957,14 +9949,14 @@
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41687</v>
       </c>
-      <c r="I3" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I3" s="32">
+        <v>0.99977762446172591</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>118</v>
       </c>
       <c r="L3" s="26">
-        <v>2.5829999999999998E-3</v>
+        <v>2.313E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -9993,14 +9985,14 @@
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41715</v>
       </c>
-      <c r="I4" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I4" s="32">
+        <v>0.99957357913449107</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>119</v>
       </c>
       <c r="L4" s="26">
-        <v>2.6029999999999998E-3</v>
+        <v>2.3189999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -10029,14 +10021,14 @@
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41746</v>
       </c>
-      <c r="I5" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I5" s="32">
+        <v>0.99933494259570266</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>120</v>
       </c>
       <c r="L5" s="26">
-        <v>2.6619999999999999E-3</v>
+        <v>2.379E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -10052,7 +10044,7 @@
       </c>
       <c r="E6" s="39">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>2.5249999999999995E-3</v>
+        <v>2.4500000000000632E-3</v>
       </c>
       <c r="F6" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -10066,20 +10058,20 @@
         <f>_xll.qlRateHelperLatestDate($D6)</f>
         <v>41778</v>
       </c>
-      <c r="I6" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I6" s="32">
+        <v>0.99915833011755029</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>121</v>
       </c>
       <c r="L6" s="26">
-        <v>2.9250000000000001E-3</v>
+        <v>2.4499999999999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_RateHelpersSelected#0008</v>
+        <v>USD_YC3MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="42" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10090,7 +10082,7 @@
       </c>
       <c r="E7" s="39">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>2.6249999999999885E-3</v>
+        <v>2.5249999999999995E-3</v>
       </c>
       <c r="F7" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -10104,14 +10096,14 @@
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41809</v>
       </c>
-      <c r="I7" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I7" s="32">
+        <v>0.99891317048737271</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>122</v>
       </c>
       <c r="L7" s="26">
-        <v>3.0249999999999999E-3</v>
+        <v>2.5249999999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -10120,7 +10112,7 @@
       </c>
       <c r="E8" s="39">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>3.0500000000001082E-3</v>
+        <v>2.9250000000000664E-3</v>
       </c>
       <c r="F8" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -10134,23 +10126,23 @@
         <f>_xll.qlRateHelperLatestDate($D8)</f>
         <v>41900</v>
       </c>
-      <c r="I8" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I8" s="32">
+        <v>0.9981755145508362</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>123</v>
       </c>
       <c r="L8" s="26">
-        <v>3.4499999999999999E-3</v>
+        <v>2.9250000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="40" t="str">
-        <v>USD_YC3MRH_FUT3MH5</v>
+        <v>USD_YC3MRH_FUT3MU4</v>
       </c>
       <c r="E9" s="39">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>4.6250000000001013E-3</v>
+        <v>3.5250000000001114E-3</v>
       </c>
       <c r="F9" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -10158,29 +10150,29 @@
       </c>
       <c r="G9" s="38">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42081</v>
+        <v>41899</v>
       </c>
       <c r="H9" s="37">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42173</v>
-      </c>
-      <c r="I9" s="32" t="e">
-        <v>#NUM!</v>
+        <v>41990</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0.99729544837494244</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="L9" s="26">
-        <v>5.1250000000000002E-3</v>
+        <v>3.5249999999999999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="40" t="str">
-        <v>USD_YC3MRH_FUT3MM5</v>
+        <v>USD_YC3MRH_FUT3MZ4</v>
       </c>
       <c r="E10" s="39">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>5.6249999999999911E-3</v>
+        <v>4.3750000000000178E-3</v>
       </c>
       <c r="F10" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -10188,29 +10180,29 @@
       </c>
       <c r="G10" s="38">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42172</v>
+        <v>41990</v>
       </c>
       <c r="H10" s="37">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42264</v>
-      </c>
-      <c r="I10" s="32" t="e">
-        <v>#NUM!</v>
+        <v>42080</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0.99620584822785907</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>125</v>
+        <v>185</v>
       </c>
       <c r="L10" s="26">
-        <v>6.025E-3</v>
+        <v>4.3750000000000004E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="40" t="str">
-        <v>USD_YC3MRH_FUT3MU5</v>
+        <v>USD_YC3MRH_FUT3MH5</v>
       </c>
       <c r="E11" s="39">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>6.8000000000000282E-3</v>
+        <v>5.6249999999999911E-3</v>
       </c>
       <c r="F11" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -10218,30 +10210,30 @@
       </c>
       <c r="G11" s="38">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42263</v>
+        <v>42081</v>
       </c>
       <c r="H11" s="37">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42354</v>
-      </c>
-      <c r="I11" s="32" t="e">
-        <v>#NUM!</v>
+        <v>42173</v>
+      </c>
+      <c r="I11" s="32">
+        <v>0.99476230831010515</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L11" s="26">
-        <v>7.2249999999999997E-3</v>
+        <v>5.6249999999999998E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="41"/>
       <c r="D12" s="40" t="str">
-        <v>USD_YC3MRH_FUT3MZ5</v>
+        <v>USD_YC3MRH_FUT3MM5</v>
       </c>
       <c r="E12" s="39">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>8.2249999999999268E-3</v>
+        <v>7.2750000000000314E-3</v>
       </c>
       <c r="F12" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -10249,30 +10241,30 @@
       </c>
       <c r="G12" s="38">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42354</v>
+        <v>42172</v>
       </c>
       <c r="H12" s="37">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42445</v>
-      </c>
-      <c r="I12" s="32" t="e">
-        <v>#NUM!</v>
+        <v>42264</v>
+      </c>
+      <c r="I12" s="32">
+        <v>0.99293399850867159</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L12" s="26">
-        <v>8.8749999999999992E-3</v>
+        <v>7.2750000000000002E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="41"/>
       <c r="D13" s="40" t="str">
-        <v>USD_YC3MRH_FUT3MH6</v>
+        <v>USD_YC3MRH_FUT3MU5</v>
       </c>
       <c r="E13" s="39">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>1.0074999999999945E-2</v>
+        <v>9.3250000000000277E-3</v>
       </c>
       <c r="F13" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10280,29 +10272,29 @@
       </c>
       <c r="G13" s="38">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42445</v>
+        <v>42263</v>
       </c>
       <c r="H13" s="37">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42537</v>
-      </c>
-      <c r="I13" s="32" t="e">
-        <v>#NUM!</v>
+        <v>42354</v>
+      </c>
+      <c r="I13" s="32">
+        <v>0.99062128528333759</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L13" s="26">
-        <v>1.0925000000000001E-2</v>
+        <v>9.325E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="40" t="str">
-        <v>USD_YC3MRH_FUT3MM6</v>
+        <v>USD_YC3MRH_FUT3MZ5</v>
       </c>
       <c r="E14" s="39">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>1.2249999999999983E-2</v>
+        <v>1.177499999999998E-2</v>
       </c>
       <c r="F14" s="39">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -10310,20 +10302,20 @@
       </c>
       <c r="G14" s="38">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42536</v>
+        <v>42354</v>
       </c>
       <c r="H14" s="37">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42628</v>
-      </c>
-      <c r="I14" s="32" t="e">
-        <v>#NUM!</v>
+        <v>42445</v>
+      </c>
+      <c r="I14" s="32">
+        <v>0.98768149247438308</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L14" s="26">
-        <v>1.325E-2</v>
+        <v>1.1775000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -10346,14 +10338,14 @@
         <f>_xll.qlRateHelperLatestDate($D15)</f>
         <v>42752</v>
       </c>
-      <c r="I15" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I15" s="32">
+        <v>0.97941235424936446</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L15" s="26">
-        <v>7.4000000000000003E-3</v>
+        <v>8.9599999999999992E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -10376,14 +10368,14 @@
         <f>_xll.qlRateHelperLatestDate($D16)</f>
         <v>43117</v>
       </c>
-      <c r="I16" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I16" s="32">
+        <v>0.95866816110103537</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L16" s="26">
-        <v>1.0999999999999999E-2</v>
+        <v>1.34E-2</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
@@ -10406,14 +10398,14 @@
         <f>_xll.qlRateHelperLatestDate($D17)</f>
         <v>43482</v>
       </c>
-      <c r="I17" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I17" s="32">
+        <v>0.93103821166076683</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L17" s="26">
-        <v>1.469E-2</v>
+        <v>1.753E-2</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
@@ -10436,14 +10428,14 @@
         <f>_xll.qlRateHelperLatestDate($D18)</f>
         <v>43847</v>
       </c>
-      <c r="I18" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I18" s="32">
+        <v>0.89901397807918926</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L18" s="26">
-        <v>1.7999999999999999E-2</v>
+        <v>2.102E-2</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
@@ -10466,14 +10458,14 @@
         <f>_xll.qlRateHelperLatestDate($D19)</f>
         <v>44214</v>
       </c>
-      <c r="I19" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I19" s="32">
+        <v>0.86507764264036835</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L19" s="26">
-        <v>2.0830000000000001E-2</v>
+        <v>2.3900000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
@@ -10496,14 +10488,14 @@
         <f>_xll.qlRateHelperLatestDate($D20)</f>
         <v>44578</v>
       </c>
-      <c r="I20" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I20" s="32">
+        <v>0.83060121832712586</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L20" s="26">
-        <v>2.3140000000000001E-2</v>
+        <v>2.6210000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
@@ -10526,14 +10518,14 @@
         <f>_xll.qlRateHelperLatestDate($D21)</f>
         <v>44943</v>
       </c>
-      <c r="I21" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I21" s="32">
+        <v>0.79611466210360604</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L21" s="26">
-        <v>2.5100000000000001E-2</v>
+        <v>2.8119999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
@@ -10556,14 +10548,14 @@
         <f>_xll.qlRateHelperLatestDate($D22)</f>
         <v>45308</v>
       </c>
-      <c r="I22" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I22" s="32">
+        <v>0.76220240340897372</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L22" s="26">
-        <v>2.6790000000000001E-2</v>
+        <v>2.9729999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
@@ -10586,14 +10578,14 @@
         <f>_xll.qlRateHelperLatestDate($D23)</f>
         <v>46041</v>
       </c>
-      <c r="I23" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I23" s="32">
+        <v>0.69638680537343678</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L23" s="26">
-        <v>2.947E-2</v>
+        <v>3.2219999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
@@ -10616,14 +10608,14 @@
         <f>_xll.qlRateHelperLatestDate($D24)</f>
         <v>47135</v>
       </c>
-      <c r="I24" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I24" s="32">
+        <v>0.60846810768332271</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L24" s="26">
-        <v>3.2009999999999997E-2</v>
+        <v>3.4599999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
@@ -10646,14 +10638,14 @@
         <f>_xll.qlRateHelperLatestDate($D25)</f>
         <v>48961</v>
       </c>
-      <c r="I25" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I25" s="32">
+        <v>0.48956523304713978</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L25" s="26">
-        <v>3.4000000000000002E-2</v>
+        <v>3.6569999999999998E-2</v>
       </c>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.2">
@@ -10676,14 +10668,14 @@
         <f>_xll.qlRateHelperLatestDate($D26)</f>
         <v>50787</v>
       </c>
-      <c r="I26" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I26" s="32">
+        <v>0.39662795867057987</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L26" s="26">
-        <v>3.4959999999999998E-2</v>
+        <v>3.7470000000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.2">
@@ -10706,14 +10698,14 @@
         <f>_xll.qlRateHelperLatestDate($D27)</f>
         <v>52614</v>
       </c>
-      <c r="I27" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I27" s="32">
+        <v>0.32340521637732628</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L27" s="26">
-        <v>3.5490000000000001E-2</v>
+        <v>3.7940000000000002E-2</v>
       </c>
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.2">
@@ -10736,14 +10728,14 @@
         <f>_xll.qlRateHelperLatestDate($D28)</f>
         <v>56268</v>
       </c>
-      <c r="I28" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I28" s="32">
+        <v>0.2252585858919666</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L28" s="26">
-        <v>3.5619999999999999E-2</v>
+        <v>3.814E-2</v>
       </c>
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.2">
@@ -10766,14 +10758,14 @@
         <f>_xll.qlRateHelperLatestDate($D29)</f>
         <v>59918</v>
       </c>
-      <c r="I29" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="I29" s="32">
+        <v>0.16094323852142145</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L29" s="26">
-        <v>3.5459999999999998E-2</v>
+        <v>3.7960000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.2">
@@ -10797,7 +10789,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I30" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.2">
@@ -10821,7 +10813,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I31" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.2">
@@ -10845,7 +10837,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I32" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
@@ -10869,7 +10861,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I33" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
@@ -10893,7 +10885,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.2">
@@ -10917,7 +10909,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.2">
@@ -10941,7 +10933,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.2">
@@ -10965,7 +10957,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I37" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.2">
@@ -10989,7 +10981,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.2">
@@ -11013,7 +11005,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.2">
@@ -11037,7 +11029,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.2">
@@ -11061,7 +11053,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.2">
@@ -11085,7 +11077,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.2">
@@ -11109,7 +11101,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.2">
@@ -11133,7 +11125,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.2">
@@ -11157,7 +11149,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.2">
@@ -11181,7 +11173,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.2">
@@ -11205,7 +11197,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.2">
@@ -11229,7 +11221,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.2">
@@ -11253,7 +11245,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.2">
@@ -11277,7 +11269,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
@@ -11301,7 +11293,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
@@ -11325,7 +11317,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
@@ -11349,7 +11341,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -11373,7 +11365,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
@@ -11397,7 +11389,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
@@ -11421,7 +11413,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
@@ -11445,7 +11437,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
@@ -11469,7 +11461,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
@@ -11493,7 +11485,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
@@ -11517,7 +11509,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
@@ -11541,7 +11533,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
@@ -11565,7 +11557,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
@@ -11589,7 +11581,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
@@ -11613,7 +11605,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.2">
@@ -11637,7 +11629,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.2">
@@ -11661,7 +11653,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.2">
@@ -11685,7 +11677,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.2">
@@ -11709,7 +11701,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.2">
@@ -11733,7 +11725,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.2">
@@ -11757,7 +11749,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.2">
@@ -11781,7 +11773,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.2">
@@ -11805,7 +11797,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.2">
@@ -11829,7 +11821,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.2">
@@ -11853,7 +11845,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.2">
@@ -11877,7 +11869,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.2">
@@ -11901,7 +11893,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.2">
@@ -11925,7 +11917,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.2">
@@ -11949,7 +11941,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.2">
@@ -11973,7 +11965,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.2">
@@ -11997,7 +11989,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="4:9" x14ac:dyDescent="0.2">
@@ -12021,7 +12013,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="4:9" x14ac:dyDescent="0.2">
@@ -12045,7 +12037,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="4:9" x14ac:dyDescent="0.2">
@@ -12069,7 +12061,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="4:9" x14ac:dyDescent="0.2">
@@ -12093,7 +12085,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="4:9" x14ac:dyDescent="0.2">
@@ -12117,7 +12109,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.2">
@@ -12141,7 +12133,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.2">
@@ -12165,7 +12157,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.2">
@@ -12189,7 +12181,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.2">
@@ -12213,7 +12205,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="4:9" x14ac:dyDescent="0.2">
@@ -12237,7 +12229,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="4:9" x14ac:dyDescent="0.2">
@@ -12261,7 +12253,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="4:9" x14ac:dyDescent="0.2">
@@ -12285,7 +12277,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.2">
@@ -12309,7 +12301,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.2">
@@ -12333,7 +12325,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.2">
@@ -12357,7 +12349,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.2">
@@ -12381,7 +12373,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
@@ -12405,7 +12397,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
@@ -12429,7 +12421,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
@@ -12453,7 +12445,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
@@ -12477,7 +12469,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
@@ -12501,7 +12493,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
@@ -12525,7 +12517,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
@@ -12549,7 +12541,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
@@ -12573,7 +12565,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
@@ -12597,7 +12589,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
@@ -12621,7 +12613,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
@@ -12645,7 +12637,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
@@ -12669,7 +12661,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
@@ -12693,7 +12685,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
@@ -12717,7 +12709,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
@@ -12741,7 +12733,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
@@ -12765,7 +12757,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="4:9" x14ac:dyDescent="0.2">
@@ -12789,7 +12781,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
@@ -12813,7 +12805,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
@@ -12837,7 +12829,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
@@ -12861,7 +12853,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
@@ -12885,7 +12877,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
@@ -12909,7 +12901,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
@@ -12933,7 +12925,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
@@ -12957,7 +12949,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
@@ -12981,7 +12973,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
@@ -13005,7 +12997,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
@@ -13029,7 +13021,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
@@ -13053,7 +13045,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
@@ -13077,7 +13069,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -13101,7 +13093,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="32" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -13125,9 +13117,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13144,12 +13134,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="112" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
       <c r="D1" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E1" s="110" t="str">
         <f>Currency&amp;"_YC"&amp;$D$1&amp;"RH"</f>
@@ -13163,10 +13153,10 @@
       <c r="A2" s="101"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E2" s="107" t="str">
         <f>$E$1&amp;"_Deposits.xml"</f>
@@ -13185,7 +13175,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="101"/>
       <c r="B3" s="104" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C3" s="103"/>
       <c r="D3" s="98" t="str">
@@ -13198,7 +13188,7 @@
       </c>
       <c r="F3" s="102" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_SND#0008</v>
+        <v>USD_YC3MRH_SND#0002</v>
       </c>
       <c r="G3" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13209,7 +13199,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="101"/>
       <c r="B4" s="100" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="99" t="str">
         <f t="shared" ref="C4:C9" si="2">PROPER(Currency)&amp;FamilyName&amp;$B4</f>
@@ -13225,7 +13215,7 @@
       </c>
       <c r="F4" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_SWD#0008</v>
+        <v>USD_YC3MRH_SWD#0002</v>
       </c>
       <c r="G4" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13236,7 +13226,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="101"/>
       <c r="B5" s="100" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="99" t="str">
         <f t="shared" si="2"/>
@@ -13252,7 +13242,7 @@
       </c>
       <c r="F5" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_2WD#0008</v>
+        <v>USD_YC3MRH_2WD#0002</v>
       </c>
       <c r="G5" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13263,7 +13253,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="101"/>
       <c r="B6" s="100" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="99" t="str">
         <f t="shared" si="2"/>
@@ -13279,7 +13269,7 @@
       </c>
       <c r="F6" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_3WD#0008</v>
+        <v>USD_YC3MRH_3WD#0002</v>
       </c>
       <c r="G6" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13290,7 +13280,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="101"/>
       <c r="B7" s="100" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="99" t="str">
         <f t="shared" si="2"/>
@@ -13306,7 +13296,7 @@
       </c>
       <c r="F7" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_1MD#0008</v>
+        <v>USD_YC3MRH_1MD#0002</v>
       </c>
       <c r="G7" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13317,7 +13307,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="101"/>
       <c r="B8" s="100" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="99" t="str">
         <f t="shared" si="2"/>
@@ -13333,7 +13323,7 @@
       </c>
       <c r="F8" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_2MD#0008</v>
+        <v>USD_YC3MRH_2MD#0002</v>
       </c>
       <c r="G8" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13344,7 +13334,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="101"/>
       <c r="B9" s="100" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C9" s="99" t="str">
         <f t="shared" si="2"/>
@@ -13360,7 +13350,7 @@
       </c>
       <c r="F9" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_3MD#0008</v>
+        <v>USD_YC3MRH_3MD#0002</v>
       </c>
       <c r="G9" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13391,7 +13381,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M4" sqref="M4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13412,13 +13402,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="144" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B1" s="148"/>
       <c r="C1" s="148"/>
       <c r="D1" s="148"/>
       <c r="E1" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F1" s="147"/>
       <c r="G1" s="147"/>
@@ -13434,22 +13424,22 @@
     <row r="2" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="144"/>
       <c r="B2" s="104" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C2" s="108" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="143" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E2" s="108" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F2" s="108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G2" s="104" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H2" s="107" t="str">
         <f>$H$1&amp;"_Futures"&amp;$E$1&amp;".xml"</f>
@@ -13495,7 +13485,7 @@
       </c>
       <c r="I3" s="141" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MF4#0008</v>
+        <v>USD_YC3MRH_FUT3MF4#0002</v>
       </c>
       <c r="J3" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -13533,7 +13523,7 @@
       </c>
       <c r="I4" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MG4#0008</v>
+        <v>USD_YC3MRH_FUT3MG4#0002</v>
       </c>
       <c r="J4" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -13543,7 +13533,7 @@
       <c r="L4" s="139"/>
       <c r="M4" s="90">
         <f>_xll.qlQuoteValue(F4)</f>
-        <v>99.747500000000002</v>
+        <v>99.754999999999995</v>
       </c>
       <c r="N4" s="90">
         <f>_xll.qlQuoteValue(G4)</f>
@@ -13551,7 +13541,7 @@
       </c>
       <c r="O4" s="90">
         <f>_xll.qlRateHelperRate(I4)</f>
-        <v>2.5249999999999995E-3</v>
+        <v>2.4500000000000632E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -13583,7 +13573,7 @@
       </c>
       <c r="I5" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH4#0008</v>
+        <v>USD_YC3MRH_FUT3MH4#0002</v>
       </c>
       <c r="J5" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13621,7 +13611,7 @@
       </c>
       <c r="I6" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MJ4#0008</v>
+        <v>USD_YC3MRH_FUT3MJ4#0002</v>
       </c>
       <c r="J6" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13659,7 +13649,7 @@
       </c>
       <c r="I7" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MK4#0008</v>
+        <v>USD_YC3MRH_FUT3MK4#0002</v>
       </c>
       <c r="J7" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -13697,7 +13687,7 @@
       </c>
       <c r="I8" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM4#0008</v>
+        <v>USD_YC3MRH_FUT3MM4#0002</v>
       </c>
       <c r="J8" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -13735,7 +13725,7 @@
       </c>
       <c r="I9" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MN4#0008</v>
+        <v>USD_YC3MRH_FUT3MN4#0002</v>
       </c>
       <c r="J9" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -13773,7 +13763,7 @@
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MQ4#0008</v>
+        <v>USD_YC3MRH_FUT3MQ4#0002</v>
       </c>
       <c r="J10" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -13811,7 +13801,7 @@
       </c>
       <c r="I11" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU4#0008</v>
+        <v>USD_YC3MRH_FUT3MU4#0002</v>
       </c>
       <c r="J11" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -13819,17 +13809,17 @@
       </c>
       <c r="K11" s="94"/>
       <c r="L11" s="139"/>
-      <c r="M11" s="90" t="e">
+      <c r="M11" s="90">
         <f>_xll.qlQuoteValue(F11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N11" s="90" t="e">
+        <v>99.647499999999994</v>
+      </c>
+      <c r="N11" s="90">
         <f>_xll.qlQuoteValue(G11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O11" s="90" t="e">
+        <v>0</v>
+      </c>
+      <c r="O11" s="90">
         <f>_xll.qlRateHelperRate(I11)</f>
-        <v>#NUM!</v>
+        <v>3.5250000000001114E-3</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -13861,7 +13851,7 @@
       </c>
       <c r="I12" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MV4#0008</v>
+        <v>USD_YC3MRH_FUT3MV4#0002</v>
       </c>
       <c r="J12" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -13899,7 +13889,7 @@
       </c>
       <c r="I13" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MX4#0008</v>
+        <v>USD_YC3MRH_FUT3MX4#0002</v>
       </c>
       <c r="J13" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -13937,7 +13927,7 @@
       </c>
       <c r="I14" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ4#0008</v>
+        <v>USD_YC3MRH_FUT3MZ4#0002</v>
       </c>
       <c r="J14" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -13975,7 +13965,7 @@
       </c>
       <c r="I15" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H15,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH5#0008</v>
+        <v>USD_YC3MRH_FUT3MH5#0002</v>
       </c>
       <c r="J15" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -14013,7 +14003,7 @@
       </c>
       <c r="I16" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H16,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM5#0008</v>
+        <v>USD_YC3MRH_FUT3MM5#0002</v>
       </c>
       <c r="J16" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -14051,7 +14041,7 @@
       </c>
       <c r="I17" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H17,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU5#0008</v>
+        <v>USD_YC3MRH_FUT3MU5#0002</v>
       </c>
       <c r="J17" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -14089,7 +14079,7 @@
       </c>
       <c r="I18" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H18,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ5#0008</v>
+        <v>USD_YC3MRH_FUT3MZ5#0002</v>
       </c>
       <c r="J18" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -14127,7 +14117,7 @@
       </c>
       <c r="I19" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H19,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH6#0008</v>
+        <v>USD_YC3MRH_FUT3MH6#0002</v>
       </c>
       <c r="J19" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -14165,7 +14155,7 @@
       </c>
       <c r="I20" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H20,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM6#0008</v>
+        <v>USD_YC3MRH_FUT3MM6#0002</v>
       </c>
       <c r="J20" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -14203,7 +14193,7 @@
       </c>
       <c r="I21" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H21,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU6#0008</v>
+        <v>USD_YC3MRH_FUT3MU6#0002</v>
       </c>
       <c r="J21" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -14241,7 +14231,7 @@
       </c>
       <c r="I22" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H22,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ6#0008</v>
+        <v>USD_YC3MRH_FUT3MZ6#0002</v>
       </c>
       <c r="J22" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -14279,7 +14269,7 @@
       </c>
       <c r="I23" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H23,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH7#0008</v>
+        <v>USD_YC3MRH_FUT3MH7#0002</v>
       </c>
       <c r="J23" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -14317,7 +14307,7 @@
       </c>
       <c r="I24" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H24,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM7#0008</v>
+        <v>USD_YC3MRH_FUT3MM7#0002</v>
       </c>
       <c r="J24" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -14355,7 +14345,7 @@
       </c>
       <c r="I25" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H25,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU7#0008</v>
+        <v>USD_YC3MRH_FUT3MU7#0002</v>
       </c>
       <c r="J25" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -14393,7 +14383,7 @@
       </c>
       <c r="I26" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H26,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ7#0008</v>
+        <v>USD_YC3MRH_FUT3MZ7#0002</v>
       </c>
       <c r="J26" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -14431,7 +14421,7 @@
       </c>
       <c r="I27" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H27,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH8#0008</v>
+        <v>USD_YC3MRH_FUT3MH8#0002</v>
       </c>
       <c r="J27" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -14469,7 +14459,7 @@
       </c>
       <c r="I28" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H28,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM8#0008</v>
+        <v>USD_YC3MRH_FUT3MM8#0002</v>
       </c>
       <c r="J28" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -14507,7 +14497,7 @@
       </c>
       <c r="I29" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H29,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU8#0008</v>
+        <v>USD_YC3MRH_FUT3MU8#0002</v>
       </c>
       <c r="J29" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -14545,7 +14535,7 @@
       </c>
       <c r="I30" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H30,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ8#0008</v>
+        <v>USD_YC3MRH_FUT3MZ8#0002</v>
       </c>
       <c r="J30" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -14583,7 +14573,7 @@
       </c>
       <c r="I31" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H31,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH9#0008</v>
+        <v>USD_YC3MRH_FUT3MH9#0002</v>
       </c>
       <c r="J31" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -14621,7 +14611,7 @@
       </c>
       <c r="I32" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H32,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM9#0008</v>
+        <v>USD_YC3MRH_FUT3MM9#0002</v>
       </c>
       <c r="J32" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -14659,7 +14649,7 @@
       </c>
       <c r="I33" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H33,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU9#0008</v>
+        <v>USD_YC3MRH_FUT3MU9#0002</v>
       </c>
       <c r="J33" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -14697,7 +14687,7 @@
       </c>
       <c r="I34" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H34,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ9#0008</v>
+        <v>USD_YC3MRH_FUT3MZ9#0002</v>
       </c>
       <c r="J34" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -14735,7 +14725,7 @@
       </c>
       <c r="I35" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H35,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH0#0008</v>
+        <v>USD_YC3MRH_FUT3MH0#0002</v>
       </c>
       <c r="J35" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -14773,7 +14763,7 @@
       </c>
       <c r="I36" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H36,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM0#0008</v>
+        <v>USD_YC3MRH_FUT3MM0#0002</v>
       </c>
       <c r="J36" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -14811,7 +14801,7 @@
       </c>
       <c r="I37" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H37,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU0#0008</v>
+        <v>USD_YC3MRH_FUT3MU0#0002</v>
       </c>
       <c r="J37" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -14849,7 +14839,7 @@
       </c>
       <c r="I38" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H38,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ0#0008</v>
+        <v>USD_YC3MRH_FUT3MZ0#0002</v>
       </c>
       <c r="J38" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -14887,7 +14877,7 @@
       </c>
       <c r="I39" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H39,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH1#0008</v>
+        <v>USD_YC3MRH_FUT3MH1#0002</v>
       </c>
       <c r="J39" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -14925,7 +14915,7 @@
       </c>
       <c r="I40" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H40,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM1#0008</v>
+        <v>USD_YC3MRH_FUT3MM1#0002</v>
       </c>
       <c r="J40" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -14962,7 +14952,7 @@
       </c>
       <c r="I41" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H41,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU1#0008</v>
+        <v>USD_YC3MRH_FUT3MU1#0002</v>
       </c>
       <c r="J41" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -14999,7 +14989,7 @@
       </c>
       <c r="I42" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H42,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ1#0008</v>
+        <v>USD_YC3MRH_FUT3MZ1#0002</v>
       </c>
       <c r="J42" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -15036,7 +15026,7 @@
       </c>
       <c r="I43" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H43,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH2#0008</v>
+        <v>USD_YC3MRH_FUT3MH2#0002</v>
       </c>
       <c r="J43" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -15073,7 +15063,7 @@
       </c>
       <c r="I44" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H44,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM2#0008</v>
+        <v>USD_YC3MRH_FUT3MM2#0002</v>
       </c>
       <c r="J44" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -15106,7 +15096,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15133,7 +15125,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="179" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B1" s="177"/>
       <c r="C1" s="177"/>
@@ -15160,7 +15152,7 @@
       <c r="H2" s="111"/>
       <c r="I2" s="111"/>
       <c r="J2" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K2" s="12" t="str">
         <f>Currency&amp;"_YC"&amp;$J$2&amp;"RH"</f>
@@ -15176,37 +15168,37 @@
     <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="101"/>
       <c r="B3" s="108" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C3" s="108"/>
       <c r="D3" s="108"/>
       <c r="E3" s="108"/>
       <c r="F3" s="108" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G3" s="108" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H3" s="108" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I3" s="108" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J3" s="108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K3" s="175" t="str">
         <f>K2&amp;"_Swaps.xml"</f>
         <v>USD_YC3MRH_Swaps.xml</v>
       </c>
-      <c r="L3" s="174" t="e">
+      <c r="L3" s="174">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(L4:L50,SerializationPath&amp;K3,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
+        <v>45</v>
       </c>
       <c r="M3" s="153" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L3)</f>
-        <v>ohObjectSave - operToVectorImpl: error converting parameter 'ObjectList' to type 'class std::basic_string&lt;char,struct std::char_traits&lt;char&gt;,class std::allocator&lt;char&gt; &gt;' : Unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'class s</v>
+        <v/>
       </c>
       <c r="N3" s="152"/>
     </row>
@@ -15227,7 +15219,7 @@
       </c>
       <c r="L4" s="172" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>USD_YC3MRH_AM3L_Libor3M#0008</v>
+        <v>USD_YC3MRH_AM3L_Libor3M#0002</v>
       </c>
       <c r="M4" s="171" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -15254,7 +15246,7 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="101"/>
       <c r="B6" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C6" s="161" t="s">
         <v>36</v>
@@ -15272,7 +15264,7 @@
         <v>Annual</v>
       </c>
       <c r="G6" s="137" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H6" s="137" t="str">
         <f t="shared" ref="H6:H42" si="1">IF(UPPER(RIGHT($D6))="B",BondBasisDayCounter,IF(UPPER(RIGHT($D6))="M",MoneyMarketDayCounter,"--"))</f>
@@ -15289,12 +15281,12 @@
         <f t="shared" ref="K6:K42" si="3">$K$2&amp;"_"&amp;$D6&amp;$E6&amp;$C6</f>
         <v>USD_YC3MRH_AM3L1Y</v>
       </c>
-      <c r="L6" s="154" t="e">
+      <c r="L6" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L1Y#0002</v>
       </c>
       <c r="M6" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L6)</f>
+        <f>_xll.ohRangeRetrieveError(L6)</f>
         <v/>
       </c>
       <c r="N6" s="152"/>
@@ -15305,13 +15297,13 @@
         <v>111</v>
       </c>
       <c r="R6" s="168" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="101"/>
       <c r="B7" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C7" s="161" t="s">
         <v>35</v>
@@ -15327,7 +15319,7 @@
         <v>Annual</v>
       </c>
       <c r="G7" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H7" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15344,12 +15336,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L15M</v>
       </c>
-      <c r="L7" s="154" t="e">
+      <c r="L7" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L15M#0002</v>
       </c>
       <c r="M7" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L7)</f>
+        <f>_xll.ohRangeRetrieveError(L7)</f>
         <v/>
       </c>
       <c r="N7" s="152"/>
@@ -15360,13 +15352,13 @@
         <v>111</v>
       </c>
       <c r="R7" s="165" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="101"/>
       <c r="B8" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C8" s="161" t="s">
         <v>34</v>
@@ -15382,7 +15374,7 @@
         <v>Annual</v>
       </c>
       <c r="G8" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H8" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15399,12 +15391,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L18M</v>
       </c>
-      <c r="L8" s="154" t="e">
+      <c r="L8" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L18M#0002</v>
       </c>
       <c r="M8" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L8)</f>
+        <f>_xll.ohRangeRetrieveError(L8)</f>
         <v/>
       </c>
       <c r="N8" s="152"/>
@@ -15415,13 +15407,13 @@
         <v>103</v>
       </c>
       <c r="R8" s="165" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="101"/>
       <c r="B9" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C9" s="161" t="s">
         <v>33</v>
@@ -15437,7 +15429,7 @@
         <v>Annual</v>
       </c>
       <c r="G9" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H9" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15454,12 +15446,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L21M</v>
       </c>
-      <c r="L9" s="154" t="e">
+      <c r="L9" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L21M#0002</v>
       </c>
       <c r="M9" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L9)</f>
+        <f>_xll.ohRangeRetrieveError(L9)</f>
         <v/>
       </c>
       <c r="N9" s="152"/>
@@ -15470,13 +15462,13 @@
         <v>108</v>
       </c>
       <c r="R9" s="165" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="101"/>
       <c r="B10" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C10" s="159" t="s">
         <v>32</v>
@@ -15492,7 +15484,7 @@
         <v>Annual</v>
       </c>
       <c r="G10" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H10" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15509,12 +15501,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L2Y</v>
       </c>
-      <c r="L10" s="154" t="e">
+      <c r="L10" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L2Y#0002</v>
       </c>
       <c r="M10" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L10)</f>
+        <f>_xll.ohRangeRetrieveError(L10)</f>
         <v/>
       </c>
       <c r="N10" s="152"/>
@@ -15525,13 +15517,13 @@
         <v>103</v>
       </c>
       <c r="R10" s="162" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="101"/>
       <c r="B11" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C11" s="159" t="s">
         <v>31</v>
@@ -15547,7 +15539,7 @@
         <v>Annual</v>
       </c>
       <c r="G11" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H11" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15564,12 +15556,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L3Y</v>
       </c>
-      <c r="L11" s="154" t="e">
+      <c r="L11" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L3Y#0002</v>
       </c>
       <c r="M11" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L11)</f>
+        <f>_xll.ohRangeRetrieveError(L11)</f>
         <v/>
       </c>
       <c r="N11" s="152"/>
@@ -15577,7 +15569,7 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="101"/>
       <c r="B12" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C12" s="159" t="s">
         <v>30</v>
@@ -15593,7 +15585,7 @@
         <v>Annual</v>
       </c>
       <c r="G12" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H12" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15610,12 +15602,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L4Y</v>
       </c>
-      <c r="L12" s="154" t="e">
+      <c r="L12" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L4Y#0002</v>
       </c>
       <c r="M12" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L12)</f>
+        <f>_xll.ohRangeRetrieveError(L12)</f>
         <v/>
       </c>
       <c r="N12" s="152"/>
@@ -15623,7 +15615,7 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="101"/>
       <c r="B13" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="159" t="s">
         <v>29</v>
@@ -15639,7 +15631,7 @@
         <v>Annual</v>
       </c>
       <c r="G13" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H13" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15656,12 +15648,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L5Y</v>
       </c>
-      <c r="L13" s="154" t="e">
+      <c r="L13" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L5Y#0002</v>
       </c>
       <c r="M13" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L13)</f>
+        <f>_xll.ohRangeRetrieveError(L13)</f>
         <v/>
       </c>
       <c r="N13" s="152"/>
@@ -15669,7 +15661,7 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="101"/>
       <c r="B14" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C14" s="159" t="s">
         <v>28</v>
@@ -15685,7 +15677,7 @@
         <v>Annual</v>
       </c>
       <c r="G14" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H14" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15702,12 +15694,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L6Y</v>
       </c>
-      <c r="L14" s="154" t="e">
+      <c r="L14" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L6Y#0002</v>
       </c>
       <c r="M14" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L14)</f>
+        <f>_xll.ohRangeRetrieveError(L14)</f>
         <v/>
       </c>
       <c r="N14" s="152"/>
@@ -15715,7 +15707,7 @@
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="101"/>
       <c r="B15" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C15" s="159" t="s">
         <v>27</v>
@@ -15731,7 +15723,7 @@
         <v>Annual</v>
       </c>
       <c r="G15" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H15" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15748,12 +15740,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L7Y</v>
       </c>
-      <c r="L15" s="154" t="e">
+      <c r="L15" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L7Y#0002</v>
       </c>
       <c r="M15" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L15)</f>
+        <f>_xll.ohRangeRetrieveError(L15)</f>
         <v/>
       </c>
       <c r="N15" s="152"/>
@@ -15761,7 +15753,7 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="101"/>
       <c r="B16" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C16" s="159" t="s">
         <v>26</v>
@@ -15777,7 +15769,7 @@
         <v>Annual</v>
       </c>
       <c r="G16" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H16" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15794,12 +15786,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L8Y</v>
       </c>
-      <c r="L16" s="154" t="e">
+      <c r="L16" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L8Y#0002</v>
       </c>
       <c r="M16" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L16)</f>
+        <f>_xll.ohRangeRetrieveError(L16)</f>
         <v/>
       </c>
       <c r="N16" s="152"/>
@@ -15807,7 +15799,7 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="101"/>
       <c r="B17" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C17" s="159" t="s">
         <v>25</v>
@@ -15823,7 +15815,7 @@
         <v>Annual</v>
       </c>
       <c r="G17" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H17" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15840,12 +15832,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L9Y</v>
       </c>
-      <c r="L17" s="154" t="e">
+      <c r="L17" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L9Y#0002</v>
       </c>
       <c r="M17" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L17)</f>
+        <f>_xll.ohRangeRetrieveError(L17)</f>
         <v/>
       </c>
       <c r="N17" s="152"/>
@@ -15853,7 +15845,7 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="101"/>
       <c r="B18" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C18" s="159" t="s">
         <v>24</v>
@@ -15869,7 +15861,7 @@
         <v>Annual</v>
       </c>
       <c r="G18" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H18" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15886,12 +15878,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L10Y</v>
       </c>
-      <c r="L18" s="154" t="e">
+      <c r="L18" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L10Y#0002</v>
       </c>
       <c r="M18" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L18)</f>
+        <f>_xll.ohRangeRetrieveError(L18)</f>
         <v/>
       </c>
       <c r="N18" s="152"/>
@@ -15899,7 +15891,7 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="101"/>
       <c r="B19" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C19" s="159" t="s">
         <v>23</v>
@@ -15915,7 +15907,7 @@
         <v>Annual</v>
       </c>
       <c r="G19" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H19" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15932,12 +15924,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L11Y</v>
       </c>
-      <c r="L19" s="154" t="e">
+      <c r="L19" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L11Y#0002</v>
       </c>
       <c r="M19" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L19)</f>
+        <f>_xll.ohRangeRetrieveError(L19)</f>
         <v/>
       </c>
       <c r="N19" s="152"/>
@@ -15945,7 +15937,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="101"/>
       <c r="B20" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C20" s="159" t="s">
         <v>22</v>
@@ -15961,7 +15953,7 @@
         <v>Annual</v>
       </c>
       <c r="G20" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H20" s="136" t="str">
         <f t="shared" si="1"/>
@@ -15978,12 +15970,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L12Y</v>
       </c>
-      <c r="L20" s="154" t="e">
+      <c r="L20" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L12Y#0002</v>
       </c>
       <c r="M20" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L20)</f>
+        <f>_xll.ohRangeRetrieveError(L20)</f>
         <v/>
       </c>
       <c r="N20" s="152"/>
@@ -15991,7 +15983,7 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="101"/>
       <c r="B21" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C21" s="159" t="s">
         <v>21</v>
@@ -16007,7 +15999,7 @@
         <v>Annual</v>
       </c>
       <c r="G21" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H21" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16024,12 +16016,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L13Y</v>
       </c>
-      <c r="L21" s="154" t="e">
+      <c r="L21" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L13Y#0002</v>
       </c>
       <c r="M21" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L21)</f>
+        <f>_xll.ohRangeRetrieveError(L21)</f>
         <v/>
       </c>
       <c r="N21" s="152"/>
@@ -16037,7 +16029,7 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="101"/>
       <c r="B22" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22" s="159" t="s">
         <v>20</v>
@@ -16053,7 +16045,7 @@
         <v>Annual</v>
       </c>
       <c r="G22" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H22" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16070,12 +16062,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L14Y</v>
       </c>
-      <c r="L22" s="154" t="e">
+      <c r="L22" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L14Y#0002</v>
       </c>
       <c r="M22" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L22)</f>
+        <f>_xll.ohRangeRetrieveError(L22)</f>
         <v/>
       </c>
       <c r="N22" s="152"/>
@@ -16083,7 +16075,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="101"/>
       <c r="B23" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C23" s="159" t="s">
         <v>19</v>
@@ -16099,7 +16091,7 @@
         <v>Annual</v>
       </c>
       <c r="G23" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H23" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16116,12 +16108,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L15Y</v>
       </c>
-      <c r="L23" s="154" t="e">
+      <c r="L23" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L15Y#0002</v>
       </c>
       <c r="M23" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L23)</f>
+        <f>_xll.ohRangeRetrieveError(L23)</f>
         <v/>
       </c>
       <c r="N23" s="152"/>
@@ -16129,7 +16121,7 @@
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="101"/>
       <c r="B24" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C24" s="159" t="s">
         <v>18</v>
@@ -16145,7 +16137,7 @@
         <v>Annual</v>
       </c>
       <c r="G24" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H24" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16162,12 +16154,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L16Y</v>
       </c>
-      <c r="L24" s="154" t="e">
+      <c r="L24" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L16Y#0002</v>
       </c>
       <c r="M24" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L24)</f>
+        <f>_xll.ohRangeRetrieveError(L24)</f>
         <v/>
       </c>
       <c r="N24" s="152"/>
@@ -16175,7 +16167,7 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="101"/>
       <c r="B25" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C25" s="159" t="s">
         <v>17</v>
@@ -16191,7 +16183,7 @@
         <v>Annual</v>
       </c>
       <c r="G25" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H25" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16208,12 +16200,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L17Y</v>
       </c>
-      <c r="L25" s="154" t="e">
+      <c r="L25" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L17Y#0002</v>
       </c>
       <c r="M25" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L25)</f>
+        <f>_xll.ohRangeRetrieveError(L25)</f>
         <v/>
       </c>
       <c r="N25" s="152"/>
@@ -16221,7 +16213,7 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="101"/>
       <c r="B26" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C26" s="159" t="s">
         <v>16</v>
@@ -16237,7 +16229,7 @@
         <v>Annual</v>
       </c>
       <c r="G26" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H26" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16254,12 +16246,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L18Y</v>
       </c>
-      <c r="L26" s="154" t="e">
+      <c r="L26" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L18Y#0002</v>
       </c>
       <c r="M26" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L26)</f>
+        <f>_xll.ohRangeRetrieveError(L26)</f>
         <v/>
       </c>
       <c r="N26" s="152"/>
@@ -16267,7 +16259,7 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="101"/>
       <c r="B27" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C27" s="159" t="s">
         <v>15</v>
@@ -16283,7 +16275,7 @@
         <v>Annual</v>
       </c>
       <c r="G27" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H27" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16300,12 +16292,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L19Y</v>
       </c>
-      <c r="L27" s="154" t="e">
+      <c r="L27" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L19Y#0002</v>
       </c>
       <c r="M27" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L27)</f>
+        <f>_xll.ohRangeRetrieveError(L27)</f>
         <v/>
       </c>
       <c r="N27" s="152"/>
@@ -16313,7 +16305,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="101"/>
       <c r="B28" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C28" s="159" t="s">
         <v>14</v>
@@ -16329,7 +16321,7 @@
         <v>Annual</v>
       </c>
       <c r="G28" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H28" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16346,12 +16338,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L20Y</v>
       </c>
-      <c r="L28" s="154" t="e">
+      <c r="L28" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L20Y#0002</v>
       </c>
       <c r="M28" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L28)</f>
+        <f>_xll.ohRangeRetrieveError(L28)</f>
         <v/>
       </c>
       <c r="N28" s="152"/>
@@ -16359,7 +16351,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="101"/>
       <c r="B29" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C29" s="159" t="s">
         <v>13</v>
@@ -16375,7 +16367,7 @@
         <v>Annual</v>
       </c>
       <c r="G29" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H29" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16392,12 +16384,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L21Y</v>
       </c>
-      <c r="L29" s="154" t="e">
+      <c r="L29" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L21Y#0002</v>
       </c>
       <c r="M29" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L29)</f>
+        <f>_xll.ohRangeRetrieveError(L29)</f>
         <v/>
       </c>
       <c r="N29" s="152"/>
@@ -16405,7 +16397,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="101"/>
       <c r="B30" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C30" s="159" t="s">
         <v>12</v>
@@ -16421,7 +16413,7 @@
         <v>Annual</v>
       </c>
       <c r="G30" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H30" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16438,12 +16430,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L22Y</v>
       </c>
-      <c r="L30" s="154" t="e">
+      <c r="L30" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L22Y#0002</v>
       </c>
       <c r="M30" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L30)</f>
+        <f>_xll.ohRangeRetrieveError(L30)</f>
         <v/>
       </c>
       <c r="N30" s="152"/>
@@ -16451,7 +16443,7 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="101"/>
       <c r="B31" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C31" s="159" t="s">
         <v>11</v>
@@ -16467,7 +16459,7 @@
         <v>Annual</v>
       </c>
       <c r="G31" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H31" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16484,12 +16476,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L23Y</v>
       </c>
-      <c r="L31" s="154" t="e">
+      <c r="L31" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L23Y#0002</v>
       </c>
       <c r="M31" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L31)</f>
+        <f>_xll.ohRangeRetrieveError(L31)</f>
         <v/>
       </c>
       <c r="N31" s="152"/>
@@ -16497,7 +16489,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="101"/>
       <c r="B32" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C32" s="159" t="s">
         <v>10</v>
@@ -16513,7 +16505,7 @@
         <v>Annual</v>
       </c>
       <c r="G32" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H32" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16530,12 +16522,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L24Y</v>
       </c>
-      <c r="L32" s="154" t="e">
+      <c r="L32" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L24Y#0002</v>
       </c>
       <c r="M32" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L32)</f>
+        <f>_xll.ohRangeRetrieveError(L32)</f>
         <v/>
       </c>
       <c r="N32" s="152"/>
@@ -16543,7 +16535,7 @@
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="101"/>
       <c r="B33" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C33" s="159" t="s">
         <v>9</v>
@@ -16559,7 +16551,7 @@
         <v>Annual</v>
       </c>
       <c r="G33" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H33" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16576,12 +16568,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L25Y</v>
       </c>
-      <c r="L33" s="154" t="e">
+      <c r="L33" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L25Y#0002</v>
       </c>
       <c r="M33" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L33)</f>
+        <f>_xll.ohRangeRetrieveError(L33)</f>
         <v/>
       </c>
       <c r="N33" s="152"/>
@@ -16589,7 +16581,7 @@
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="101"/>
       <c r="B34" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C34" s="159" t="s">
         <v>8</v>
@@ -16605,7 +16597,7 @@
         <v>Annual</v>
       </c>
       <c r="G34" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H34" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16622,12 +16614,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L26Y</v>
       </c>
-      <c r="L34" s="154" t="e">
+      <c r="L34" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L26Y#0002</v>
       </c>
       <c r="M34" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L34)</f>
+        <f>_xll.ohRangeRetrieveError(L34)</f>
         <v/>
       </c>
       <c r="N34" s="152"/>
@@ -16635,7 +16627,7 @@
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="101"/>
       <c r="B35" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C35" s="159" t="s">
         <v>7</v>
@@ -16651,7 +16643,7 @@
         <v>Annual</v>
       </c>
       <c r="G35" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H35" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16668,12 +16660,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L27Y</v>
       </c>
-      <c r="L35" s="154" t="e">
+      <c r="L35" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L27Y#0002</v>
       </c>
       <c r="M35" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L35)</f>
+        <f>_xll.ohRangeRetrieveError(L35)</f>
         <v/>
       </c>
       <c r="N35" s="152"/>
@@ -16681,7 +16673,7 @@
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="101"/>
       <c r="B36" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C36" s="159" t="s">
         <v>6</v>
@@ -16697,7 +16689,7 @@
         <v>Annual</v>
       </c>
       <c r="G36" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H36" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16714,12 +16706,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L28Y</v>
       </c>
-      <c r="L36" s="154" t="e">
+      <c r="L36" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L28Y#0002</v>
       </c>
       <c r="M36" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L36)</f>
+        <f>_xll.ohRangeRetrieveError(L36)</f>
         <v/>
       </c>
       <c r="N36" s="152"/>
@@ -16727,7 +16719,7 @@
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="101"/>
       <c r="B37" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C37" s="159" t="s">
         <v>5</v>
@@ -16743,7 +16735,7 @@
         <v>Annual</v>
       </c>
       <c r="G37" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H37" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16760,12 +16752,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L29Y</v>
       </c>
-      <c r="L37" s="154" t="e">
+      <c r="L37" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L29Y#0002</v>
       </c>
       <c r="M37" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L37)</f>
+        <f>_xll.ohRangeRetrieveError(L37)</f>
         <v/>
       </c>
       <c r="N37" s="152"/>
@@ -16773,7 +16765,7 @@
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="101"/>
       <c r="B38" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C38" s="159" t="s">
         <v>4</v>
@@ -16789,7 +16781,7 @@
         <v>Annual</v>
       </c>
       <c r="G38" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H38" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16806,12 +16798,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L30Y</v>
       </c>
-      <c r="L38" s="154" t="e">
+      <c r="L38" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L30Y#0002</v>
       </c>
       <c r="M38" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L38)</f>
+        <f>_xll.ohRangeRetrieveError(L38)</f>
         <v/>
       </c>
       <c r="N38" s="152"/>
@@ -16819,7 +16811,7 @@
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="101"/>
       <c r="B39" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" s="159" t="s">
         <v>3</v>
@@ -16835,7 +16827,7 @@
         <v>Annual</v>
       </c>
       <c r="G39" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H39" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16852,12 +16844,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L35Y</v>
       </c>
-      <c r="L39" s="154" t="e">
+      <c r="L39" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L35Y#0002</v>
       </c>
       <c r="M39" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L39)</f>
+        <f>_xll.ohRangeRetrieveError(L39)</f>
         <v/>
       </c>
       <c r="N39" s="152"/>
@@ -16865,7 +16857,7 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="101"/>
       <c r="B40" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C40" s="159" t="s">
         <v>2</v>
@@ -16881,7 +16873,7 @@
         <v>Annual</v>
       </c>
       <c r="G40" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H40" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16898,12 +16890,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L40Y</v>
       </c>
-      <c r="L40" s="154" t="e">
+      <c r="L40" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L40Y#0002</v>
       </c>
       <c r="M40" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L40)</f>
+        <f>_xll.ohRangeRetrieveError(L40)</f>
         <v/>
       </c>
       <c r="N40" s="152"/>
@@ -16911,7 +16903,7 @@
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="101"/>
       <c r="B41" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C41" s="159" t="s">
         <v>1</v>
@@ -16927,7 +16919,7 @@
         <v>Annual</v>
       </c>
       <c r="G41" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H41" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16944,12 +16936,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L50Y</v>
       </c>
-      <c r="L41" s="154" t="e">
+      <c r="L41" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L50Y#0002</v>
       </c>
       <c r="M41" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L41)</f>
+        <f>_xll.ohRangeRetrieveError(L41)</f>
         <v/>
       </c>
       <c r="N41" s="152"/>
@@ -16957,7 +16949,7 @@
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="101"/>
       <c r="B42" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C42" s="159" t="s">
         <v>0</v>
@@ -16973,7 +16965,7 @@
         <v>Annual</v>
       </c>
       <c r="G42" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H42" s="136" t="str">
         <f t="shared" si="1"/>
@@ -16990,12 +16982,12 @@
         <f t="shared" si="3"/>
         <v>USD_YC3MRH_AM3L60Y</v>
       </c>
-      <c r="L42" s="154" t="e">
+      <c r="L42" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_AM3L60Y#0002</v>
       </c>
       <c r="M42" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L42)</f>
+        <f>_xll.ohRangeRetrieveError(L42)</f>
         <v/>
       </c>
       <c r="N42" s="152"/>
@@ -17019,7 +17011,7 @@
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="101"/>
       <c r="B44" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C44" s="161"/>
       <c r="D44" s="158" t="s">
@@ -17029,13 +17021,13 @@
         <v>12</v>
       </c>
       <c r="F44" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G44" s="137" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H44" s="137" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I44" s="157">
         <v>0</v>
@@ -17048,12 +17040,12 @@
         <f t="shared" ref="K44:K50" si="5">$K$2&amp;"_"&amp;$D44&amp;$E44&amp;$C44</f>
         <v>USD_YC3MRH_1S12</v>
       </c>
-      <c r="L44" s="154" t="e">
+      <c r="L44" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_1S12#0002</v>
       </c>
       <c r="M44" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L44)</f>
+        <f>_xll.ohRangeRetrieveError(L44)</f>
         <v/>
       </c>
       <c r="N44" s="152"/>
@@ -17064,7 +17056,7 @@
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="101"/>
       <c r="B45" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C45" s="159"/>
       <c r="D45" s="158" t="s">
@@ -17074,13 +17066,13 @@
         <v>12</v>
       </c>
       <c r="F45" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G45" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H45" s="136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I45" s="157">
         <v>0</v>
@@ -17093,12 +17085,12 @@
         <f t="shared" si="5"/>
         <v>USD_YC3MRH_2S12</v>
       </c>
-      <c r="L45" s="154" t="e">
+      <c r="L45" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_2S12#0002</v>
       </c>
       <c r="M45" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L45)</f>
+        <f>_xll.ohRangeRetrieveError(L45)</f>
         <v/>
       </c>
       <c r="N45" s="152"/>
@@ -17109,7 +17101,7 @@
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="101"/>
       <c r="B46" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C46" s="159"/>
       <c r="D46" s="158" t="s">
@@ -17119,13 +17111,13 @@
         <v>12</v>
       </c>
       <c r="F46" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G46" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H46" s="136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I46" s="157">
         <v>0</v>
@@ -17138,12 +17130,12 @@
         <f t="shared" si="5"/>
         <v>USD_YC3MRH_3S12</v>
       </c>
-      <c r="L46" s="154" t="e">
+      <c r="L46" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_3S12#0002</v>
       </c>
       <c r="M46" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L46)</f>
+        <f>_xll.ohRangeRetrieveError(L46)</f>
         <v/>
       </c>
       <c r="N46" s="152"/>
@@ -17154,7 +17146,7 @@
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="101"/>
       <c r="B47" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C47" s="159"/>
       <c r="D47" s="158" t="s">
@@ -17164,13 +17156,13 @@
         <v>12</v>
       </c>
       <c r="F47" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G47" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H47" s="136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I47" s="157">
         <v>0</v>
@@ -17183,12 +17175,12 @@
         <f t="shared" si="5"/>
         <v>USD_YC3MRH_4S12</v>
       </c>
-      <c r="L47" s="154" t="e">
+      <c r="L47" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_4S12#0002</v>
       </c>
       <c r="M47" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L47)</f>
+        <f>_xll.ohRangeRetrieveError(L47)</f>
         <v/>
       </c>
       <c r="N47" s="152"/>
@@ -17199,7 +17191,7 @@
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="101"/>
       <c r="B48" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C48" s="159"/>
       <c r="D48" s="158" t="s">
@@ -17209,13 +17201,13 @@
         <v>24</v>
       </c>
       <c r="F48" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G48" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H48" s="136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I48" s="157">
         <v>0</v>
@@ -17228,12 +17220,12 @@
         <f t="shared" si="5"/>
         <v>USD_YC3MRH_1S24</v>
       </c>
-      <c r="L48" s="154" t="e">
+      <c r="L48" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_1S24#0002</v>
       </c>
       <c r="M48" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L48)</f>
+        <f>_xll.ohRangeRetrieveError(L48)</f>
         <v/>
       </c>
       <c r="N48" s="152"/>
@@ -17244,7 +17236,7 @@
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="101"/>
       <c r="B49" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C49" s="159"/>
       <c r="D49" s="158" t="s">
@@ -17254,13 +17246,13 @@
         <v>24</v>
       </c>
       <c r="F49" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G49" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H49" s="136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I49" s="157">
         <v>0</v>
@@ -17273,12 +17265,12 @@
         <f t="shared" si="5"/>
         <v>USD_YC3MRH_2S24</v>
       </c>
-      <c r="L49" s="154" t="e">
+      <c r="L49" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_2S24#0002</v>
       </c>
       <c r="M49" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L49)</f>
+        <f>_xll.ohRangeRetrieveError(L49)</f>
         <v/>
       </c>
       <c r="N49" s="152"/>
@@ -17289,7 +17281,7 @@
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="101"/>
       <c r="B50" s="158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C50" s="159"/>
       <c r="D50" s="158" t="s">
@@ -17299,13 +17291,13 @@
         <v>36</v>
       </c>
       <c r="F50" s="158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G50" s="136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H50" s="136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I50" s="157">
         <v>0</v>
@@ -17318,12 +17310,12 @@
         <f t="shared" si="5"/>
         <v>USD_YC3MRH_1S36</v>
       </c>
-      <c r="L50" s="154" t="e">
+      <c r="L50" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#VALUE!</v>
+        <v>USD_YC3MRH_1S36#0002</v>
       </c>
       <c r="M50" s="153" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L50)</f>
+        <f>_xll.ohRangeRetrieveError(L50)</f>
         <v/>
       </c>
       <c r="N50" s="152"/>

</xml_diff>

<commit_message>
USD 3M YC - fix triggers
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YC3MBootstrapping.xlsx
@@ -809,6 +809,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -865,6 +866,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -879,6 +881,7 @@
       <sz val="12"/>
       <color indexed="16"/>
       <name val="MS Sans Serif"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -894,6 +897,7 @@
       <sz val="8"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2355,7 +2359,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="85">
-        <v>41654.758842592593</v>
+        <v>41655.66741898148</v>
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="56"/>
@@ -2409,7 +2413,7 @@
       </c>
       <c r="D14" s="82" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYC3M#0002</v>
+        <v>_USDYC3M#0001</v>
       </c>
       <c r="E14" s="57"/>
       <c r="F14" s="56"/>
@@ -2603,7 +2607,7 @@
       </c>
       <c r="D28" s="61">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.16094323852142145</v>
+        <v>0.16094246296918882</v>
       </c>
       <c r="E28" s="57"/>
       <c r="F28" s="56"/>
@@ -2671,9 +2675,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2816,7 +2818,7 @@
       </c>
       <c r="F4" s="13">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>2.611E-3</v>
+        <v>2.3010000000000001E-3</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="12" t="b">
@@ -2855,7 +2857,7 @@
       </c>
       <c r="F5" s="13">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>2.6090000000000002E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="12" t="b">
@@ -2894,7 +2896,7 @@
       </c>
       <c r="F6" s="13">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>2.5969999999999999E-3</v>
+        <v>2.2980000000000001E-3</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="12" t="b">
@@ -2933,7 +2935,7 @@
       </c>
       <c r="F7" s="13">
         <f>_xll.qlRateHelperQuoteValue($E7,Trigger)</f>
-        <v>2.5850000000000001E-3</v>
+        <v>2.3059999999999999E-3</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="12" t="b">
@@ -2972,7 +2974,7 @@
       </c>
       <c r="F8" s="13">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
-        <v>2.5829999999999998E-3</v>
+        <v>2.313E-3</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="12" t="b">
@@ -3011,7 +3013,7 @@
       </c>
       <c r="F9" s="13">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
-        <v>2.6029999999999998E-3</v>
+        <v>2.3189999999999999E-3</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="12" t="b">
@@ -3044,7 +3046,7 @@
       </c>
       <c r="F10" s="13">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
-        <v>2.6619999999999999E-3</v>
+        <v>2.379E-3</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="12" t="b">
@@ -4008,15 +4010,15 @@
       </c>
       <c r="E36" s="14" t="str">
         <f>'3M_Futures'!I3</f>
-        <v>USD_YC3MRH_FUT3MF4#0002</v>
-      </c>
-      <c r="F36" s="28">
+        <v>USD_YC3MRH_FUT3MF4#0000</v>
+      </c>
+      <c r="F36" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
-        <v>99.758749999999992</v>
-      </c>
-      <c r="G36" s="13">
+        <v>#NUM!</v>
+      </c>
+      <c r="G36" s="13" t="e">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E36,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="H36" s="12" t="b">
         <v>1</v>
@@ -4053,7 +4055,7 @@
       </c>
       <c r="E37" s="14" t="str">
         <f>'3M_Futures'!I4</f>
-        <v>USD_YC3MRH_FUT3MG4#0002</v>
+        <v>USD_YC3MRH_FUT3MG4#0000</v>
       </c>
       <c r="F37" s="28">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -4098,7 +4100,7 @@
       </c>
       <c r="E38" s="14" t="str">
         <f>'3M_Futures'!I5</f>
-        <v>USD_YC3MRH_FUT3MH4#0002</v>
+        <v>USD_YC3MRH_FUT3MH4#0000</v>
       </c>
       <c r="F38" s="28">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -4143,7 +4145,7 @@
       </c>
       <c r="E39" s="14" t="str">
         <f>'3M_Futures'!I6</f>
-        <v>USD_YC3MRH_FUT3MJ4#0002</v>
+        <v>USD_YC3MRH_FUT3MJ4#0000</v>
       </c>
       <c r="F39" s="28">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4188,7 +4190,7 @@
       </c>
       <c r="E40" s="14" t="str">
         <f>'3M_Futures'!I7</f>
-        <v>USD_YC3MRH_FUT3MK4#0002</v>
+        <v>USD_YC3MRH_FUT3MK4#0000</v>
       </c>
       <c r="F40" s="28">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4233,7 +4235,7 @@
       </c>
       <c r="E41" s="14" t="str">
         <f>'3M_Futures'!I8</f>
-        <v>USD_YC3MRH_FUT3MM4#0002</v>
+        <v>USD_YC3MRH_FUT3MM4#0000</v>
       </c>
       <c r="F41" s="28">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4278,7 +4280,7 @@
       </c>
       <c r="E42" s="14" t="str">
         <f>'3M_Futures'!I9</f>
-        <v>USD_YC3MRH_FUT3MN4#0002</v>
+        <v>USD_YC3MRH_FUT3MN4#0000</v>
       </c>
       <c r="F42" s="28">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4323,15 +4325,15 @@
       </c>
       <c r="E43" s="14" t="str">
         <f>'3M_Futures'!I10</f>
-        <v>USD_YC3MRH_FUT3MQ4#0002</v>
-      </c>
-      <c r="F43" s="28">
+        <v>USD_YC3MRH_FUT3MQ4#0000</v>
+      </c>
+      <c r="F43" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
-        <v>99.662499999999994</v>
-      </c>
-      <c r="G43" s="13">
+        <v>#NUM!</v>
+      </c>
+      <c r="G43" s="13" t="e">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E43,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="H43" s="12" t="b">
         <v>1</v>
@@ -4368,7 +4370,7 @@
       </c>
       <c r="E44" s="14" t="str">
         <f>'3M_Futures'!I11</f>
-        <v>USD_YC3MRH_FUT3MU4#0002</v>
+        <v>USD_YC3MRH_FUT3MU4#0000</v>
       </c>
       <c r="F44" s="28">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4413,7 +4415,7 @@
       </c>
       <c r="E45" s="14" t="str">
         <f>'3M_Futures'!I12</f>
-        <v>USD_YC3MRH_FUT3MV4#0002</v>
+        <v>USD_YC3MRH_FUT3MV4#0000</v>
       </c>
       <c r="F45" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4458,15 +4460,15 @@
       </c>
       <c r="E46" s="14" t="str">
         <f>'3M_Futures'!I13</f>
-        <v>USD_YC3MRH_FUT3MX4#0002</v>
-      </c>
-      <c r="F46" s="28">
+        <v>USD_YC3MRH_FUT3MX4#0000</v>
+      </c>
+      <c r="F46" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
-        <v>99.612499999999997</v>
-      </c>
-      <c r="G46" s="13">
+        <v>#NUM!</v>
+      </c>
+      <c r="G46" s="13" t="e">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E46,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="H46" s="12" t="b">
         <v>1</v>
@@ -4503,7 +4505,7 @@
       </c>
       <c r="E47" s="14" t="str">
         <f>'3M_Futures'!I14</f>
-        <v>USD_YC3MRH_FUT3MZ4#0002</v>
+        <v>USD_YC3MRH_FUT3MZ4#0000</v>
       </c>
       <c r="F47" s="28">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -4548,7 +4550,7 @@
       </c>
       <c r="E48" s="14" t="str">
         <f>'3M_Futures'!I15</f>
-        <v>USD_YC3MRH_FUT3MH5#0002</v>
+        <v>USD_YC3MRH_FUT3MH5#0000</v>
       </c>
       <c r="F48" s="28">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
@@ -4593,7 +4595,7 @@
       </c>
       <c r="E49" s="14" t="str">
         <f>'3M_Futures'!I16</f>
-        <v>USD_YC3MRH_FUT3MM5#0002</v>
+        <v>USD_YC3MRH_FUT3MM5#0000</v>
       </c>
       <c r="F49" s="28">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
@@ -4638,7 +4640,7 @@
       </c>
       <c r="E50" s="14" t="str">
         <f>'3M_Futures'!I17</f>
-        <v>USD_YC3MRH_FUT3MU5#0002</v>
+        <v>USD_YC3MRH_FUT3MU5#0000</v>
       </c>
       <c r="F50" s="28">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
@@ -4683,7 +4685,7 @@
       </c>
       <c r="E51" s="14" t="str">
         <f>'3M_Futures'!I18</f>
-        <v>USD_YC3MRH_FUT3MZ5#0002</v>
+        <v>USD_YC3MRH_FUT3MZ5#0000</v>
       </c>
       <c r="F51" s="28">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
@@ -4728,7 +4730,7 @@
       </c>
       <c r="E52" s="14" t="str">
         <f>'3M_Futures'!I19</f>
-        <v>USD_YC3MRH_FUT3MH6#0002</v>
+        <v>USD_YC3MRH_FUT3MH6#0000</v>
       </c>
       <c r="F52" s="28">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
@@ -4773,7 +4775,7 @@
       </c>
       <c r="E53" s="14" t="str">
         <f>'3M_Futures'!I20</f>
-        <v>USD_YC3MRH_FUT3MM6#0002</v>
+        <v>USD_YC3MRH_FUT3MM6#0000</v>
       </c>
       <c r="F53" s="28">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
@@ -4818,7 +4820,7 @@
       </c>
       <c r="E54" s="14" t="str">
         <f>'3M_Futures'!I21</f>
-        <v>USD_YC3MRH_FUT3MU6#0002</v>
+        <v>USD_YC3MRH_FUT3MU6#0000</v>
       </c>
       <c r="F54" s="28">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
@@ -4863,7 +4865,7 @@
       </c>
       <c r="E55" s="14" t="str">
         <f>'3M_Futures'!I22</f>
-        <v>USD_YC3MRH_FUT3MZ6#0002</v>
+        <v>USD_YC3MRH_FUT3MZ6#0000</v>
       </c>
       <c r="F55" s="28">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
@@ -4908,7 +4910,7 @@
       </c>
       <c r="E56" s="14" t="str">
         <f>'3M_Futures'!I23</f>
-        <v>USD_YC3MRH_FUT3MH7#0002</v>
+        <v>USD_YC3MRH_FUT3MH7#0000</v>
       </c>
       <c r="F56" s="28">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
@@ -4953,7 +4955,7 @@
       </c>
       <c r="E57" s="14" t="str">
         <f>'3M_Futures'!I24</f>
-        <v>USD_YC3MRH_FUT3MM7#0002</v>
+        <v>USD_YC3MRH_FUT3MM7#0000</v>
       </c>
       <c r="F57" s="28">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
@@ -4998,7 +5000,7 @@
       </c>
       <c r="E58" s="14" t="str">
         <f>'3M_Futures'!I25</f>
-        <v>USD_YC3MRH_FUT3MU7#0002</v>
+        <v>USD_YC3MRH_FUT3MU7#0000</v>
       </c>
       <c r="F58" s="28">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
@@ -5043,7 +5045,7 @@
       </c>
       <c r="E59" s="14" t="str">
         <f>'3M_Futures'!I26</f>
-        <v>USD_YC3MRH_FUT3MZ7#0002</v>
+        <v>USD_YC3MRH_FUT3MZ7#0000</v>
       </c>
       <c r="F59" s="28">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
@@ -5088,7 +5090,7 @@
       </c>
       <c r="E60" s="14" t="str">
         <f>'3M_Futures'!I27</f>
-        <v>USD_YC3MRH_FUT3MH8#0002</v>
+        <v>USD_YC3MRH_FUT3MH8#0000</v>
       </c>
       <c r="F60" s="28">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
@@ -5133,7 +5135,7 @@
       </c>
       <c r="E61" s="14" t="str">
         <f>'3M_Futures'!I28</f>
-        <v>USD_YC3MRH_FUT3MM8#0002</v>
+        <v>USD_YC3MRH_FUT3MM8#0000</v>
       </c>
       <c r="F61" s="28">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
@@ -5178,7 +5180,7 @@
       </c>
       <c r="E62" s="14" t="str">
         <f>'3M_Futures'!I29</f>
-        <v>USD_YC3MRH_FUT3MU8#0002</v>
+        <v>USD_YC3MRH_FUT3MU8#0000</v>
       </c>
       <c r="F62" s="28">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
@@ -5223,7 +5225,7 @@
       </c>
       <c r="E63" s="14" t="str">
         <f>'3M_Futures'!I30</f>
-        <v>USD_YC3MRH_FUT3MZ8#0002</v>
+        <v>USD_YC3MRH_FUT3MZ8#0000</v>
       </c>
       <c r="F63" s="28">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
@@ -5268,7 +5270,7 @@
       </c>
       <c r="E64" s="14" t="str">
         <f>'3M_Futures'!I31</f>
-        <v>USD_YC3MRH_FUT3MH9#0002</v>
+        <v>USD_YC3MRH_FUT3MH9#0000</v>
       </c>
       <c r="F64" s="28">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
@@ -5313,7 +5315,7 @@
       </c>
       <c r="E65" s="14" t="str">
         <f>'3M_Futures'!I32</f>
-        <v>USD_YC3MRH_FUT3MM9#0002</v>
+        <v>USD_YC3MRH_FUT3MM9#0000</v>
       </c>
       <c r="F65" s="28">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
@@ -5358,7 +5360,7 @@
       </c>
       <c r="E66" s="14" t="str">
         <f>'3M_Futures'!I33</f>
-        <v>USD_YC3MRH_FUT3MU9#0002</v>
+        <v>USD_YC3MRH_FUT3MU9#0000</v>
       </c>
       <c r="F66" s="28">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
@@ -5403,7 +5405,7 @@
       </c>
       <c r="E67" s="14" t="str">
         <f>'3M_Futures'!I34</f>
-        <v>USD_YC3MRH_FUT3MZ9#0002</v>
+        <v>USD_YC3MRH_FUT3MZ9#0000</v>
       </c>
       <c r="F67" s="28">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
@@ -5448,7 +5450,7 @@
       </c>
       <c r="E68" s="14" t="str">
         <f>'3M_Futures'!I35</f>
-        <v>USD_YC3MRH_FUT3MH0#0002</v>
+        <v>USD_YC3MRH_FUT3MH0#0000</v>
       </c>
       <c r="F68" s="28">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
@@ -5493,7 +5495,7 @@
       </c>
       <c r="E69" s="14" t="str">
         <f>'3M_Futures'!I36</f>
-        <v>USD_YC3MRH_FUT3MM0#0002</v>
+        <v>USD_YC3MRH_FUT3MM0#0000</v>
       </c>
       <c r="F69" s="28">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
@@ -5538,7 +5540,7 @@
       </c>
       <c r="E70" s="14" t="str">
         <f>'3M_Futures'!I37</f>
-        <v>USD_YC3MRH_FUT3MU0#0002</v>
+        <v>USD_YC3MRH_FUT3MU0#0000</v>
       </c>
       <c r="F70" s="28">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
@@ -5583,7 +5585,7 @@
       </c>
       <c r="E71" s="14" t="str">
         <f>'3M_Futures'!I38</f>
-        <v>USD_YC3MRH_FUT3MZ0#0002</v>
+        <v>USD_YC3MRH_FUT3MZ0#0000</v>
       </c>
       <c r="F71" s="28">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
@@ -5628,7 +5630,7 @@
       </c>
       <c r="E72" s="14" t="str">
         <f>'3M_Futures'!I39</f>
-        <v>USD_YC3MRH_FUT3MH1#0002</v>
+        <v>USD_YC3MRH_FUT3MH1#0000</v>
       </c>
       <c r="F72" s="28">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
@@ -5673,7 +5675,7 @@
       </c>
       <c r="E73" s="14" t="str">
         <f>'3M_Futures'!I40</f>
-        <v>USD_YC3MRH_FUT3MM1#0002</v>
+        <v>USD_YC3MRH_FUT3MM1#0000</v>
       </c>
       <c r="F73" s="28">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
@@ -5718,7 +5720,7 @@
       </c>
       <c r="E74" s="14" t="str">
         <f>'3M_Futures'!I41</f>
-        <v>USD_YC3MRH_FUT3MU1#0002</v>
+        <v>USD_YC3MRH_FUT3MU1#0000</v>
       </c>
       <c r="F74" s="28">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
@@ -5763,7 +5765,7 @@
       </c>
       <c r="E75" s="14" t="str">
         <f>'3M_Futures'!I42</f>
-        <v>USD_YC3MRH_FUT3MZ1#0002</v>
+        <v>USD_YC3MRH_FUT3MZ1#0000</v>
       </c>
       <c r="F75" s="28">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
@@ -5808,7 +5810,7 @@
       </c>
       <c r="E76" s="14" t="str">
         <f>'3M_Futures'!I43</f>
-        <v>USD_YC3MRH_FUT3MH2#0002</v>
+        <v>USD_YC3MRH_FUT3MH2#0000</v>
       </c>
       <c r="F76" s="28">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
@@ -5853,7 +5855,7 @@
       </c>
       <c r="E77" s="7" t="str">
         <f>'3M_Futures'!I44</f>
-        <v>USD_YC3MRH_FUT3MM2#0002</v>
+        <v>USD_YC3MRH_FUT3MM2#0000</v>
       </c>
       <c r="F77" s="27">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
@@ -9899,7 +9901,7 @@
       </c>
       <c r="E2" s="39">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>2.6090000000000002E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="F2" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -9914,7 +9916,7 @@
         <v>41663</v>
       </c>
       <c r="I2" s="32">
-        <v>0.99994927201790285</v>
+        <v>0.99995527977776533</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>117</v>
@@ -9935,7 +9937,7 @@
       </c>
       <c r="E3" s="39">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>2.5829999999999998E-3</v>
+        <v>2.313E-3</v>
       </c>
       <c r="F3" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -9950,7 +9952,7 @@
         <v>41687</v>
       </c>
       <c r="I3" s="32">
-        <v>0.99977762446172591</v>
+        <v>0.99980086466277596</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>118</v>
@@ -9971,7 +9973,7 @@
       </c>
       <c r="E4" s="39">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>2.6029999999999998E-3</v>
+        <v>2.3189999999999999E-3</v>
       </c>
       <c r="F4" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -9986,7 +9988,7 @@
         <v>41715</v>
       </c>
       <c r="I4" s="32">
-        <v>0.99957357913449107</v>
+        <v>0.99962008605612207</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>119</v>
@@ -10007,7 +10009,7 @@
       </c>
       <c r="E5" s="39">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>2.6619999999999999E-3</v>
+        <v>2.379E-3</v>
       </c>
       <c r="F5" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -10022,7 +10024,7 @@
         <v>41746</v>
       </c>
       <c r="I5" s="32">
-        <v>0.99933494259570266</v>
+        <v>0.99940560351730812</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>120</v>
@@ -10059,7 +10061,7 @@
         <v>41778</v>
       </c>
       <c r="I6" s="32">
-        <v>0.99915833011755029</v>
+        <v>0.99918287425768681</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>121</v>
@@ -10071,7 +10073,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_RateHelpersSelected#0002</v>
+        <v>USD_YC3MRH_RateHelpersSelected#0001</v>
       </c>
       <c r="B7" s="42" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10097,7 +10099,7 @@
         <v>41809</v>
       </c>
       <c r="I7" s="32">
-        <v>0.99891317048737271</v>
+        <v>0.99896208267600384</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>122</v>
@@ -10127,7 +10129,7 @@
         <v>41900</v>
       </c>
       <c r="I8" s="32">
-        <v>0.9981755145508362</v>
+        <v>0.99822323232196308</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>123</v>
@@ -10157,7 +10159,7 @@
         <v>41990</v>
       </c>
       <c r="I9" s="32">
-        <v>0.99729544837494244</v>
+        <v>0.99734344110486095</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>184</v>
@@ -10187,7 +10189,7 @@
         <v>42080</v>
       </c>
       <c r="I10" s="32">
-        <v>0.99620584822785907</v>
+        <v>0.99625378852314095</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>185</v>
@@ -10217,7 +10219,7 @@
         <v>42173</v>
       </c>
       <c r="I11" s="32">
-        <v>0.99476230831010515</v>
+        <v>0.99481015580655319</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>124</v>
@@ -10248,7 +10250,7 @@
         <v>42264</v>
       </c>
       <c r="I12" s="32">
-        <v>0.99293399850867159</v>
+        <v>0.99298175112692899</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>125</v>
@@ -10279,7 +10281,7 @@
         <v>42354</v>
       </c>
       <c r="I13" s="32">
-        <v>0.99062128528333759</v>
+        <v>0.99066893146064172</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>126</v>
@@ -10309,7 +10311,7 @@
         <v>42445</v>
       </c>
       <c r="I14" s="32">
-        <v>0.98768149247438308</v>
+        <v>0.98772899725568508</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>127</v>
@@ -10339,7 +10341,7 @@
         <v>42752</v>
       </c>
       <c r="I15" s="32">
-        <v>0.97941235424936446</v>
+        <v>0.97941168247830535</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>128</v>
@@ -10369,7 +10371,7 @@
         <v>43117</v>
       </c>
       <c r="I16" s="32">
-        <v>0.95866816110103537</v>
+        <v>0.95866715227603283</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>129</v>
@@ -10399,7 +10401,7 @@
         <v>43482</v>
       </c>
       <c r="I17" s="32">
-        <v>0.93103821166076683</v>
+        <v>0.93103687005383928</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>130</v>
@@ -10429,7 +10431,7 @@
         <v>43847</v>
       </c>
       <c r="I18" s="32">
-        <v>0.89901397807918926</v>
+        <v>0.89901234881410608</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>131</v>
@@ -10459,7 +10461,7 @@
         <v>44214</v>
       </c>
       <c r="I19" s="32">
-        <v>0.86507764264036835</v>
+        <v>0.86507578949740604</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>132</v>
@@ -10489,7 +10491,7 @@
         <v>44578</v>
       </c>
       <c r="I20" s="32">
-        <v>0.83060121832712586</v>
+        <v>0.8305991959775515</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>133</v>
@@ -10519,7 +10521,7 @@
         <v>44943</v>
       </c>
       <c r="I21" s="32">
-        <v>0.79611466210360604</v>
+        <v>0.79611251590665388</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>134</v>
@@ -10549,7 +10551,7 @@
         <v>45308</v>
       </c>
       <c r="I22" s="32">
-        <v>0.76220240340897372</v>
+        <v>0.76220017080050217</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>135</v>
@@ -10579,7 +10581,7 @@
         <v>46041</v>
       </c>
       <c r="I23" s="32">
-        <v>0.69638680537343678</v>
+        <v>0.69638448008630371</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>136</v>
@@ -10609,7 +10611,7 @@
         <v>47135</v>
       </c>
       <c r="I24" s="32">
-        <v>0.60846810768332271</v>
+        <v>0.60846579353891606</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>137</v>
@@ -10639,7 +10641,7 @@
         <v>48961</v>
       </c>
       <c r="I25" s="32">
-        <v>0.48956523304713978</v>
+        <v>0.48956312689740528</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>138</v>
@@ -10669,7 +10671,7 @@
         <v>50787</v>
       </c>
       <c r="I26" s="32">
-        <v>0.39662795867057987</v>
+        <v>0.39662612358610461</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>139</v>
@@ -10699,7 +10701,7 @@
         <v>52614</v>
       </c>
       <c r="I27" s="32">
-        <v>0.32340521637732628</v>
+        <v>0.32340364861180199</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>140</v>
@@ -10729,7 +10731,7 @@
         <v>56268</v>
       </c>
       <c r="I28" s="32">
-        <v>0.2252585858919666</v>
+        <v>0.22525747946060301</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>141</v>
@@ -10759,7 +10761,7 @@
         <v>59918</v>
       </c>
       <c r="I29" s="32">
-        <v>0.16094323852142145</v>
+        <v>0.16094246296918882</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>142</v>
@@ -13188,7 +13190,7 @@
       </c>
       <c r="F3" s="102" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_SND#0002</v>
+        <v>USD_YC3MRH_SND#0000</v>
       </c>
       <c r="G3" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13215,7 +13217,7 @@
       </c>
       <c r="F4" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_SWD#0002</v>
+        <v>USD_YC3MRH_SWD#0000</v>
       </c>
       <c r="G4" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13242,7 +13244,7 @@
       </c>
       <c r="F5" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_2WD#0002</v>
+        <v>USD_YC3MRH_2WD#0000</v>
       </c>
       <c r="G5" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13269,7 +13271,7 @@
       </c>
       <c r="F6" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_3WD#0002</v>
+        <v>USD_YC3MRH_3WD#0000</v>
       </c>
       <c r="G6" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13296,7 +13298,7 @@
       </c>
       <c r="F7" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_1MD#0002</v>
+        <v>USD_YC3MRH_1MD#0000</v>
       </c>
       <c r="G7" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13323,7 +13325,7 @@
       </c>
       <c r="F8" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_2MD#0002</v>
+        <v>USD_YC3MRH_2MD#0000</v>
       </c>
       <c r="G8" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13350,7 +13352,7 @@
       </c>
       <c r="F9" s="96" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_3MD#0002</v>
+        <v>USD_YC3MRH_3MD#0000</v>
       </c>
       <c r="G9" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13485,7 +13487,7 @@
       </c>
       <c r="I3" s="141" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MF4#0002</v>
+        <v>USD_YC3MRH_FUT3MF4#0000</v>
       </c>
       <c r="J3" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -13523,7 +13525,7 @@
       </c>
       <c r="I4" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MG4#0002</v>
+        <v>USD_YC3MRH_FUT3MG4#0000</v>
       </c>
       <c r="J4" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -13573,7 +13575,7 @@
       </c>
       <c r="I5" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH4#0002</v>
+        <v>USD_YC3MRH_FUT3MH4#0000</v>
       </c>
       <c r="J5" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13611,7 +13613,7 @@
       </c>
       <c r="I6" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MJ4#0002</v>
+        <v>USD_YC3MRH_FUT3MJ4#0000</v>
       </c>
       <c r="J6" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13649,7 +13651,7 @@
       </c>
       <c r="I7" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MK4#0002</v>
+        <v>USD_YC3MRH_FUT3MK4#0000</v>
       </c>
       <c r="J7" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -13687,7 +13689,7 @@
       </c>
       <c r="I8" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM4#0002</v>
+        <v>USD_YC3MRH_FUT3MM4#0000</v>
       </c>
       <c r="J8" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -13725,7 +13727,7 @@
       </c>
       <c r="I9" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MN4#0002</v>
+        <v>USD_YC3MRH_FUT3MN4#0000</v>
       </c>
       <c r="J9" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -13763,7 +13765,7 @@
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MQ4#0002</v>
+        <v>USD_YC3MRH_FUT3MQ4#0000</v>
       </c>
       <c r="J10" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -13801,7 +13803,7 @@
       </c>
       <c r="I11" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU4#0002</v>
+        <v>USD_YC3MRH_FUT3MU4#0000</v>
       </c>
       <c r="J11" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -13851,7 +13853,7 @@
       </c>
       <c r="I12" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MV4#0002</v>
+        <v>USD_YC3MRH_FUT3MV4#0000</v>
       </c>
       <c r="J12" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -13889,7 +13891,7 @@
       </c>
       <c r="I13" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MX4#0002</v>
+        <v>USD_YC3MRH_FUT3MX4#0000</v>
       </c>
       <c r="J13" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -13927,7 +13929,7 @@
       </c>
       <c r="I14" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ4#0002</v>
+        <v>USD_YC3MRH_FUT3MZ4#0000</v>
       </c>
       <c r="J14" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -13965,7 +13967,7 @@
       </c>
       <c r="I15" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H15,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH5#0002</v>
+        <v>USD_YC3MRH_FUT3MH5#0000</v>
       </c>
       <c r="J15" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -14003,7 +14005,7 @@
       </c>
       <c r="I16" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H16,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM5#0002</v>
+        <v>USD_YC3MRH_FUT3MM5#0000</v>
       </c>
       <c r="J16" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -14041,7 +14043,7 @@
       </c>
       <c r="I17" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H17,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU5#0002</v>
+        <v>USD_YC3MRH_FUT3MU5#0000</v>
       </c>
       <c r="J17" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -14079,7 +14081,7 @@
       </c>
       <c r="I18" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H18,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ5#0002</v>
+        <v>USD_YC3MRH_FUT3MZ5#0000</v>
       </c>
       <c r="J18" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -14117,7 +14119,7 @@
       </c>
       <c r="I19" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H19,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH6#0002</v>
+        <v>USD_YC3MRH_FUT3MH6#0000</v>
       </c>
       <c r="J19" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -14155,7 +14157,7 @@
       </c>
       <c r="I20" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H20,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM6#0002</v>
+        <v>USD_YC3MRH_FUT3MM6#0000</v>
       </c>
       <c r="J20" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -14193,7 +14195,7 @@
       </c>
       <c r="I21" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H21,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU6#0002</v>
+        <v>USD_YC3MRH_FUT3MU6#0000</v>
       </c>
       <c r="J21" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -14231,7 +14233,7 @@
       </c>
       <c r="I22" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H22,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ6#0002</v>
+        <v>USD_YC3MRH_FUT3MZ6#0000</v>
       </c>
       <c r="J22" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -14269,7 +14271,7 @@
       </c>
       <c r="I23" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H23,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH7#0002</v>
+        <v>USD_YC3MRH_FUT3MH7#0000</v>
       </c>
       <c r="J23" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -14307,7 +14309,7 @@
       </c>
       <c r="I24" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H24,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM7#0002</v>
+        <v>USD_YC3MRH_FUT3MM7#0000</v>
       </c>
       <c r="J24" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -14345,7 +14347,7 @@
       </c>
       <c r="I25" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H25,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU7#0002</v>
+        <v>USD_YC3MRH_FUT3MU7#0000</v>
       </c>
       <c r="J25" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -14383,7 +14385,7 @@
       </c>
       <c r="I26" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H26,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ7#0002</v>
+        <v>USD_YC3MRH_FUT3MZ7#0000</v>
       </c>
       <c r="J26" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -14421,7 +14423,7 @@
       </c>
       <c r="I27" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H27,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH8#0002</v>
+        <v>USD_YC3MRH_FUT3MH8#0000</v>
       </c>
       <c r="J27" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -14459,7 +14461,7 @@
       </c>
       <c r="I28" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H28,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM8#0002</v>
+        <v>USD_YC3MRH_FUT3MM8#0000</v>
       </c>
       <c r="J28" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -14497,7 +14499,7 @@
       </c>
       <c r="I29" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H29,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU8#0002</v>
+        <v>USD_YC3MRH_FUT3MU8#0000</v>
       </c>
       <c r="J29" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -14535,7 +14537,7 @@
       </c>
       <c r="I30" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H30,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ8#0002</v>
+        <v>USD_YC3MRH_FUT3MZ8#0000</v>
       </c>
       <c r="J30" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -14573,7 +14575,7 @@
       </c>
       <c r="I31" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H31,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH9#0002</v>
+        <v>USD_YC3MRH_FUT3MH9#0000</v>
       </c>
       <c r="J31" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -14611,7 +14613,7 @@
       </c>
       <c r="I32" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H32,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM9#0002</v>
+        <v>USD_YC3MRH_FUT3MM9#0000</v>
       </c>
       <c r="J32" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -14649,7 +14651,7 @@
       </c>
       <c r="I33" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H33,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU9#0002</v>
+        <v>USD_YC3MRH_FUT3MU9#0000</v>
       </c>
       <c r="J33" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -14687,7 +14689,7 @@
       </c>
       <c r="I34" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H34,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ9#0002</v>
+        <v>USD_YC3MRH_FUT3MZ9#0000</v>
       </c>
       <c r="J34" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -14725,7 +14727,7 @@
       </c>
       <c r="I35" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H35,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH0#0002</v>
+        <v>USD_YC3MRH_FUT3MH0#0000</v>
       </c>
       <c r="J35" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -14763,7 +14765,7 @@
       </c>
       <c r="I36" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H36,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM0#0002</v>
+        <v>USD_YC3MRH_FUT3MM0#0000</v>
       </c>
       <c r="J36" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -14801,7 +14803,7 @@
       </c>
       <c r="I37" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H37,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU0#0002</v>
+        <v>USD_YC3MRH_FUT3MU0#0000</v>
       </c>
       <c r="J37" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -14839,7 +14841,7 @@
       </c>
       <c r="I38" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H38,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ0#0002</v>
+        <v>USD_YC3MRH_FUT3MZ0#0000</v>
       </c>
       <c r="J38" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -14877,7 +14879,7 @@
       </c>
       <c r="I39" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H39,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH1#0002</v>
+        <v>USD_YC3MRH_FUT3MH1#0000</v>
       </c>
       <c r="J39" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -14915,7 +14917,7 @@
       </c>
       <c r="I40" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H40,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM1#0002</v>
+        <v>USD_YC3MRH_FUT3MM1#0000</v>
       </c>
       <c r="J40" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -14952,7 +14954,7 @@
       </c>
       <c r="I41" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H41,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MU1#0002</v>
+        <v>USD_YC3MRH_FUT3MU1#0000</v>
       </c>
       <c r="J41" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -14989,7 +14991,7 @@
       </c>
       <c r="I42" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H42,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MZ1#0002</v>
+        <v>USD_YC3MRH_FUT3MZ1#0000</v>
       </c>
       <c r="J42" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -15026,7 +15028,7 @@
       </c>
       <c r="I43" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H43,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MH2#0002</v>
+        <v>USD_YC3MRH_FUT3MH2#0000</v>
       </c>
       <c r="J43" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -15063,7 +15065,7 @@
       </c>
       <c r="I44" s="134" t="str">
         <f>_xll.qlFuturesRateHelper(H44,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_FUT3MM2#0002</v>
+        <v>USD_YC3MRH_FUT3MM2#0000</v>
       </c>
       <c r="J44" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -15219,7 +15221,7 @@
       </c>
       <c r="L4" s="172" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>USD_YC3MRH_AM3L_Libor3M#0002</v>
+        <v>USD_YC3MRH_AM3L_Libor3M#0000</v>
       </c>
       <c r="M4" s="171" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -15283,7 +15285,7 @@
       </c>
       <c r="L6" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L1Y#0002</v>
+        <v>USD_YC3MRH_AM3L1Y#0000</v>
       </c>
       <c r="M6" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -15338,7 +15340,7 @@
       </c>
       <c r="L7" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L15M#0002</v>
+        <v>USD_YC3MRH_AM3L15M#0000</v>
       </c>
       <c r="M7" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -15393,7 +15395,7 @@
       </c>
       <c r="L8" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L18M#0002</v>
+        <v>USD_YC3MRH_AM3L18M#0000</v>
       </c>
       <c r="M8" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -15448,7 +15450,7 @@
       </c>
       <c r="L9" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L21M#0002</v>
+        <v>USD_YC3MRH_AM3L21M#0000</v>
       </c>
       <c r="M9" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -15503,7 +15505,7 @@
       </c>
       <c r="L10" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L2Y#0002</v>
+        <v>USD_YC3MRH_AM3L2Y#0000</v>
       </c>
       <c r="M10" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -15558,7 +15560,7 @@
       </c>
       <c r="L11" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L3Y#0002</v>
+        <v>USD_YC3MRH_AM3L3Y#0000</v>
       </c>
       <c r="M11" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -15604,7 +15606,7 @@
       </c>
       <c r="L12" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L4Y#0002</v>
+        <v>USD_YC3MRH_AM3L4Y#0000</v>
       </c>
       <c r="M12" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -15650,7 +15652,7 @@
       </c>
       <c r="L13" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L5Y#0002</v>
+        <v>USD_YC3MRH_AM3L5Y#0000</v>
       </c>
       <c r="M13" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -15696,7 +15698,7 @@
       </c>
       <c r="L14" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L6Y#0002</v>
+        <v>USD_YC3MRH_AM3L6Y#0000</v>
       </c>
       <c r="M14" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -15742,7 +15744,7 @@
       </c>
       <c r="L15" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L7Y#0002</v>
+        <v>USD_YC3MRH_AM3L7Y#0000</v>
       </c>
       <c r="M15" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -15788,7 +15790,7 @@
       </c>
       <c r="L16" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L8Y#0002</v>
+        <v>USD_YC3MRH_AM3L8Y#0000</v>
       </c>
       <c r="M16" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -15834,7 +15836,7 @@
       </c>
       <c r="L17" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L9Y#0002</v>
+        <v>USD_YC3MRH_AM3L9Y#0000</v>
       </c>
       <c r="M17" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -15880,7 +15882,7 @@
       </c>
       <c r="L18" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L10Y#0002</v>
+        <v>USD_YC3MRH_AM3L10Y#0000</v>
       </c>
       <c r="M18" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -15926,7 +15928,7 @@
       </c>
       <c r="L19" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L11Y#0002</v>
+        <v>USD_YC3MRH_AM3L11Y#0000</v>
       </c>
       <c r="M19" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -15972,7 +15974,7 @@
       </c>
       <c r="L20" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L12Y#0002</v>
+        <v>USD_YC3MRH_AM3L12Y#0000</v>
       </c>
       <c r="M20" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -16018,7 +16020,7 @@
       </c>
       <c r="L21" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L13Y#0002</v>
+        <v>USD_YC3MRH_AM3L13Y#0000</v>
       </c>
       <c r="M21" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -16064,7 +16066,7 @@
       </c>
       <c r="L22" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L14Y#0002</v>
+        <v>USD_YC3MRH_AM3L14Y#0000</v>
       </c>
       <c r="M22" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -16110,7 +16112,7 @@
       </c>
       <c r="L23" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L15Y#0002</v>
+        <v>USD_YC3MRH_AM3L15Y#0000</v>
       </c>
       <c r="M23" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -16156,7 +16158,7 @@
       </c>
       <c r="L24" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L16Y#0002</v>
+        <v>USD_YC3MRH_AM3L16Y#0000</v>
       </c>
       <c r="M24" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -16202,7 +16204,7 @@
       </c>
       <c r="L25" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L17Y#0002</v>
+        <v>USD_YC3MRH_AM3L17Y#0000</v>
       </c>
       <c r="M25" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -16248,7 +16250,7 @@
       </c>
       <c r="L26" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L18Y#0002</v>
+        <v>USD_YC3MRH_AM3L18Y#0000</v>
       </c>
       <c r="M26" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -16294,7 +16296,7 @@
       </c>
       <c r="L27" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L19Y#0002</v>
+        <v>USD_YC3MRH_AM3L19Y#0000</v>
       </c>
       <c r="M27" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -16340,7 +16342,7 @@
       </c>
       <c r="L28" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L20Y#0002</v>
+        <v>USD_YC3MRH_AM3L20Y#0000</v>
       </c>
       <c r="M28" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -16386,7 +16388,7 @@
       </c>
       <c r="L29" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L21Y#0002</v>
+        <v>USD_YC3MRH_AM3L21Y#0000</v>
       </c>
       <c r="M29" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -16432,7 +16434,7 @@
       </c>
       <c r="L30" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L22Y#0002</v>
+        <v>USD_YC3MRH_AM3L22Y#0000</v>
       </c>
       <c r="M30" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -16478,7 +16480,7 @@
       </c>
       <c r="L31" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L23Y#0002</v>
+        <v>USD_YC3MRH_AM3L23Y#0000</v>
       </c>
       <c r="M31" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -16524,7 +16526,7 @@
       </c>
       <c r="L32" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L24Y#0002</v>
+        <v>USD_YC3MRH_AM3L24Y#0000</v>
       </c>
       <c r="M32" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -16570,7 +16572,7 @@
       </c>
       <c r="L33" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L25Y#0002</v>
+        <v>USD_YC3MRH_AM3L25Y#0000</v>
       </c>
       <c r="M33" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -16616,7 +16618,7 @@
       </c>
       <c r="L34" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L26Y#0002</v>
+        <v>USD_YC3MRH_AM3L26Y#0000</v>
       </c>
       <c r="M34" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -16662,7 +16664,7 @@
       </c>
       <c r="L35" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L27Y#0002</v>
+        <v>USD_YC3MRH_AM3L27Y#0000</v>
       </c>
       <c r="M35" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -16708,7 +16710,7 @@
       </c>
       <c r="L36" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L28Y#0002</v>
+        <v>USD_YC3MRH_AM3L28Y#0000</v>
       </c>
       <c r="M36" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -16754,7 +16756,7 @@
       </c>
       <c r="L37" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L29Y#0002</v>
+        <v>USD_YC3MRH_AM3L29Y#0000</v>
       </c>
       <c r="M37" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -16800,7 +16802,7 @@
       </c>
       <c r="L38" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L30Y#0002</v>
+        <v>USD_YC3MRH_AM3L30Y#0000</v>
       </c>
       <c r="M38" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -16846,7 +16848,7 @@
       </c>
       <c r="L39" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L35Y#0002</v>
+        <v>USD_YC3MRH_AM3L35Y#0000</v>
       </c>
       <c r="M39" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -16892,7 +16894,7 @@
       </c>
       <c r="L40" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L40Y#0002</v>
+        <v>USD_YC3MRH_AM3L40Y#0000</v>
       </c>
       <c r="M40" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -16938,7 +16940,7 @@
       </c>
       <c r="L41" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L50Y#0002</v>
+        <v>USD_YC3MRH_AM3L50Y#0000</v>
       </c>
       <c r="M41" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -16984,7 +16986,7 @@
       </c>
       <c r="L42" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_AM3L60Y#0002</v>
+        <v>USD_YC3MRH_AM3L60Y#0000</v>
       </c>
       <c r="M42" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -17042,7 +17044,7 @@
       </c>
       <c r="L44" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_1S12#0002</v>
+        <v>USD_YC3MRH_1S12#0000</v>
       </c>
       <c r="M44" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -17087,7 +17089,7 @@
       </c>
       <c r="L45" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_2S12#0002</v>
+        <v>USD_YC3MRH_2S12#0000</v>
       </c>
       <c r="M45" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -17132,7 +17134,7 @@
       </c>
       <c r="L46" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_3S12#0002</v>
+        <v>USD_YC3MRH_3S12#0000</v>
       </c>
       <c r="M46" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -17177,7 +17179,7 @@
       </c>
       <c r="L47" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_4S12#0002</v>
+        <v>USD_YC3MRH_4S12#0000</v>
       </c>
       <c r="M47" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -17222,7 +17224,7 @@
       </c>
       <c r="L48" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_1S24#0002</v>
+        <v>USD_YC3MRH_1S24#0000</v>
       </c>
       <c r="M48" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -17267,7 +17269,7 @@
       </c>
       <c r="L49" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_2S24#0002</v>
+        <v>USD_YC3MRH_2S24#0000</v>
       </c>
       <c r="M49" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -17312,7 +17314,7 @@
       </c>
       <c r="L50" s="154" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC3MRH_1S36#0002</v>
+        <v>USD_YC3MRH_1S36#0000</v>
       </c>
       <c r="M50" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>

</xml_diff>